<commit_message>
them answers to part 2
</commit_message>
<xml_diff>
--- a/Auto MPG Data (1).xlsx
+++ b/Auto MPG Data (1).xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kris Capao\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9615"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$F$1</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>mpg: continuous</t>
   </si>
@@ -47,26 +43,83 @@
     <t>displacement: continuous</t>
   </si>
   <si>
-    <t>H</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
-    <t>D</t>
+    <t>SUMMARY OUTPUT</t>
   </si>
   <si>
-    <t>C</t>
+    <t>Regression Statistics</t>
   </si>
   <si>
-    <t>E</t>
+    <t>Multiple R</t>
+  </si>
+  <si>
+    <t>R Square</t>
+  </si>
+  <si>
+    <t>Adjusted R Square</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>Residual</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>Significance F</t>
+  </si>
+  <si>
+    <t>Coefficients</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>Lower 95%</t>
+  </si>
+  <si>
+    <t>Upper 95%</t>
+  </si>
+  <si>
+    <t>Lower 95.0%</t>
+  </si>
+  <si>
+    <t>Upper 95.0%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +132,14 @@
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -88,7 +149,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -96,14 +157,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -165,7 +254,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -200,7 +289,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -377,21 +466,295 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F399"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1"/>
+    <row r="3" spans="1:9">
+      <c r="A3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.84046134576780773</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.70637527372983455</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.70486563503435817</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2">
+        <v>4.2401694676444297</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="3">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2">
+        <v>16825.148031907906</v>
+      </c>
+      <c r="D12" s="2">
+        <v>8412.5740159539528</v>
+      </c>
+      <c r="E12" s="2">
+        <v>467.91015349994615</v>
+      </c>
+      <c r="F12" s="2">
+        <v>3.0596062997981754E-104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2">
+        <v>389</v>
+      </c>
+      <c r="C13" s="2">
+        <v>6993.8454374798348</v>
+      </c>
+      <c r="D13" s="2">
+        <v>17.979037114344049</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="3">
+        <v>391</v>
+      </c>
+      <c r="C14" s="3">
+        <v>23818.99346938774</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1"/>
+    <row r="16" spans="1:9">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="2">
+        <v>45.640210840177133</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.79319583288847684</v>
+      </c>
+      <c r="D17" s="2">
+        <v>57.539650295407107</v>
+      </c>
+      <c r="E17" s="2">
+        <v>2.3171132314999371E-192</v>
+      </c>
+      <c r="F17" s="2">
+        <v>44.080723592273671</v>
+      </c>
+      <c r="G17" s="2">
+        <v>47.199698088080595</v>
+      </c>
+      <c r="H17" s="2">
+        <v>44.080723592273671</v>
+      </c>
+      <c r="I17" s="2">
+        <v>47.199698088080595</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="2">
+        <v>-4.7302863086191742E-2</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1.1085086484199227E-2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>-4.2672525066554625</v>
+      </c>
+      <c r="E18" s="2">
+        <v>2.4884820102637677E-5</v>
+      </c>
+      <c r="F18" s="2">
+        <v>-6.9097040888492778E-2</v>
+      </c>
+      <c r="G18" s="2">
+        <v>-2.5508685283890699E-2</v>
+      </c>
+      <c r="H18" s="2">
+        <v>-6.9097040888492778E-2</v>
+      </c>
+      <c r="I18" s="2">
+        <v>-2.5508685283890699E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="3">
+        <v>-5.7941573648029199E-3</v>
+      </c>
+      <c r="C19" s="3">
+        <v>5.02326996413777E-4</v>
+      </c>
+      <c r="D19" s="3">
+        <v>-11.534632632067726</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1.1243623609700345E-26</v>
+      </c>
+      <c r="F19" s="3">
+        <v>-6.7817729229081979E-3</v>
+      </c>
+      <c r="G19" s="3">
+        <v>-4.806541806697642E-3</v>
+      </c>
+      <c r="H19" s="3">
+        <v>-6.7817729229081979E-3</v>
+      </c>
+      <c r="I19" s="3">
+        <v>-4.806541806697642E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F399"/>
+  <sheetViews>
+    <sheetView topLeftCell="A364" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -417,8 +780,8 @@
       <c r="A2" s="1">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
+      <c r="B2">
+        <v>1</v>
       </c>
       <c r="C2">
         <v>193</v>
@@ -437,8 +800,8 @@
       <c r="A3" s="1">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
+      <c r="B3">
+        <v>1</v>
       </c>
       <c r="C3">
         <v>215</v>
@@ -457,8 +820,8 @@
       <c r="A4" s="1">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
+      <c r="B4">
+        <v>1</v>
       </c>
       <c r="C4">
         <v>200</v>
@@ -477,8 +840,8 @@
       <c r="A5" s="1">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
-        <v>6</v>
+      <c r="B5">
+        <v>1</v>
       </c>
       <c r="C5">
         <v>210</v>
@@ -497,8 +860,8 @@
       <c r="A6" s="1">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
-        <v>6</v>
+      <c r="B6">
+        <v>1</v>
       </c>
       <c r="C6">
         <v>208</v>
@@ -517,8 +880,8 @@
       <c r="A7" s="1">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
-        <v>6</v>
+      <c r="B7">
+        <v>1</v>
       </c>
       <c r="C7">
         <v>150</v>
@@ -537,8 +900,8 @@
       <c r="A8" s="1">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
-        <v>6</v>
+      <c r="B8">
+        <v>1</v>
       </c>
       <c r="C8">
         <v>180</v>
@@ -557,8 +920,8 @@
       <c r="A9" s="1">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
-        <v>6</v>
+      <c r="B9">
+        <v>1</v>
       </c>
       <c r="C9">
         <v>180</v>
@@ -577,8 +940,8 @@
       <c r="A10" s="1">
         <v>12</v>
       </c>
-      <c r="B10" t="s">
-        <v>6</v>
+      <c r="B10">
+        <v>1</v>
       </c>
       <c r="C10">
         <v>160</v>
@@ -597,8 +960,8 @@
       <c r="A11" s="1">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
-        <v>6</v>
+      <c r="B11">
+        <v>1</v>
       </c>
       <c r="C11">
         <v>198</v>
@@ -617,8 +980,8 @@
       <c r="A12" s="1">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
-        <v>6</v>
+      <c r="B12">
+        <v>1</v>
       </c>
       <c r="C12">
         <v>225</v>
@@ -637,8 +1000,8 @@
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>6</v>
+      <c r="B13">
+        <v>1</v>
       </c>
       <c r="C13">
         <v>167</v>
@@ -657,8 +1020,8 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
-        <v>6</v>
+      <c r="B14">
+        <v>1</v>
       </c>
       <c r="C14">
         <v>180</v>
@@ -677,8 +1040,8 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
-        <v>6</v>
+      <c r="B15">
+        <v>1</v>
       </c>
       <c r="C15">
         <v>170</v>
@@ -697,8 +1060,8 @@
       <c r="A16" s="1">
         <v>13</v>
       </c>
-      <c r="B16" t="s">
-        <v>6</v>
+      <c r="B16">
+        <v>1</v>
       </c>
       <c r="C16">
         <v>175</v>
@@ -717,8 +1080,8 @@
       <c r="A17" s="1">
         <v>13</v>
       </c>
-      <c r="B17" t="s">
-        <v>6</v>
+      <c r="B17">
+        <v>1</v>
       </c>
       <c r="C17">
         <v>165</v>
@@ -737,8 +1100,8 @@
       <c r="A18" s="1">
         <v>13</v>
       </c>
-      <c r="B18" t="s">
-        <v>6</v>
+      <c r="B18">
+        <v>1</v>
       </c>
       <c r="C18">
         <v>155</v>
@@ -757,8 +1120,8 @@
       <c r="A19" s="1">
         <v>13</v>
       </c>
-      <c r="B19" t="s">
-        <v>6</v>
+      <c r="B19">
+        <v>1</v>
       </c>
       <c r="C19">
         <v>190</v>
@@ -777,8 +1140,8 @@
       <c r="A20" s="1">
         <v>13</v>
       </c>
-      <c r="B20" t="s">
-        <v>6</v>
+      <c r="B20">
+        <v>1</v>
       </c>
       <c r="C20">
         <v>130</v>
@@ -797,8 +1160,8 @@
       <c r="A21" s="1">
         <v>13</v>
       </c>
-      <c r="B21" t="s">
-        <v>6</v>
+      <c r="B21">
+        <v>1</v>
       </c>
       <c r="C21">
         <v>140</v>
@@ -817,8 +1180,8 @@
       <c r="A22" s="1">
         <v>13</v>
       </c>
-      <c r="B22" t="s">
-        <v>6</v>
+      <c r="B22">
+        <v>1</v>
       </c>
       <c r="C22">
         <v>175</v>
@@ -837,8 +1200,8 @@
       <c r="A23" s="1">
         <v>13</v>
       </c>
-      <c r="B23" t="s">
-        <v>6</v>
+      <c r="B23">
+        <v>1</v>
       </c>
       <c r="C23">
         <v>145</v>
@@ -857,8 +1220,8 @@
       <c r="A24" s="1">
         <v>13</v>
       </c>
-      <c r="B24" t="s">
-        <v>6</v>
+      <c r="B24">
+        <v>1</v>
       </c>
       <c r="C24">
         <v>150</v>
@@ -877,8 +1240,8 @@
       <c r="A25" s="1">
         <v>13</v>
       </c>
-      <c r="B25" t="s">
-        <v>6</v>
+      <c r="B25">
+        <v>1</v>
       </c>
       <c r="C25">
         <v>158</v>
@@ -897,8 +1260,8 @@
       <c r="A26" s="1">
         <v>13</v>
       </c>
-      <c r="B26" t="s">
-        <v>6</v>
+      <c r="B26">
+        <v>1</v>
       </c>
       <c r="C26">
         <v>215</v>
@@ -917,8 +1280,8 @@
       <c r="A27" s="1">
         <v>13</v>
       </c>
-      <c r="B27" t="s">
-        <v>6</v>
+      <c r="B27">
+        <v>1</v>
       </c>
       <c r="C27">
         <v>175</v>
@@ -937,8 +1300,8 @@
       <c r="A28" s="1">
         <v>13</v>
       </c>
-      <c r="B28" t="s">
-        <v>6</v>
+      <c r="B28">
+        <v>1</v>
       </c>
       <c r="C28">
         <v>170</v>
@@ -957,8 +1320,8 @@
       <c r="A29" s="1">
         <v>13</v>
       </c>
-      <c r="B29" t="s">
-        <v>6</v>
+      <c r="B29">
+        <v>1</v>
       </c>
       <c r="C29">
         <v>150</v>
@@ -977,8 +1340,8 @@
       <c r="A30" s="1">
         <v>13</v>
       </c>
-      <c r="B30" t="s">
-        <v>6</v>
+      <c r="B30">
+        <v>1</v>
       </c>
       <c r="C30">
         <v>129</v>
@@ -997,8 +1360,8 @@
       <c r="A31" s="1">
         <v>13</v>
       </c>
-      <c r="B31" t="s">
-        <v>6</v>
+      <c r="B31">
+        <v>1</v>
       </c>
       <c r="C31">
         <v>150</v>
@@ -1017,8 +1380,8 @@
       <c r="A32" s="1">
         <v>13</v>
       </c>
-      <c r="B32" t="s">
-        <v>6</v>
+      <c r="B32">
+        <v>1</v>
       </c>
       <c r="C32">
         <v>145</v>
@@ -1037,8 +1400,8 @@
       <c r="A33" s="1">
         <v>13</v>
       </c>
-      <c r="B33" t="s">
-        <v>6</v>
+      <c r="B33">
+        <v>1</v>
       </c>
       <c r="C33">
         <v>130</v>
@@ -1057,8 +1420,8 @@
       <c r="A34" s="1">
         <v>13</v>
       </c>
-      <c r="B34" t="s">
-        <v>6</v>
+      <c r="B34">
+        <v>1</v>
       </c>
       <c r="C34">
         <v>150</v>
@@ -1077,8 +1440,8 @@
       <c r="A35" s="1">
         <v>14</v>
       </c>
-      <c r="B35" t="s">
-        <v>6</v>
+      <c r="B35">
+        <v>1</v>
       </c>
       <c r="C35">
         <v>220</v>
@@ -1097,8 +1460,8 @@
       <c r="A36" s="1">
         <v>14</v>
       </c>
-      <c r="B36" t="s">
-        <v>6</v>
+      <c r="B36">
+        <v>1</v>
       </c>
       <c r="C36">
         <v>215</v>
@@ -1117,8 +1480,8 @@
       <c r="A37" s="1">
         <v>14</v>
       </c>
-      <c r="B37" t="s">
-        <v>6</v>
+      <c r="B37">
+        <v>1</v>
       </c>
       <c r="C37">
         <v>225</v>
@@ -1137,8 +1500,8 @@
       <c r="A38" s="1">
         <v>14</v>
       </c>
-      <c r="B38" t="s">
-        <v>6</v>
+      <c r="B38">
+        <v>1</v>
       </c>
       <c r="C38">
         <v>160</v>
@@ -1157,8 +1520,8 @@
       <c r="A39" s="1">
         <v>14</v>
       </c>
-      <c r="B39" t="s">
-        <v>6</v>
+      <c r="B39">
+        <v>1</v>
       </c>
       <c r="C39">
         <v>225</v>
@@ -1177,8 +1540,8 @@
       <c r="A40" s="1">
         <v>14</v>
       </c>
-      <c r="B40" t="s">
-        <v>6</v>
+      <c r="B40">
+        <v>1</v>
       </c>
       <c r="C40">
         <v>165</v>
@@ -1197,8 +1560,8 @@
       <c r="A41" s="1">
         <v>14</v>
       </c>
-      <c r="B41" t="s">
-        <v>6</v>
+      <c r="B41">
+        <v>1</v>
       </c>
       <c r="C41">
         <v>175</v>
@@ -1217,8 +1580,8 @@
       <c r="A42" s="1">
         <v>14</v>
       </c>
-      <c r="B42" t="s">
-        <v>6</v>
+      <c r="B42">
+        <v>1</v>
       </c>
       <c r="C42">
         <v>153</v>
@@ -1237,8 +1600,8 @@
       <c r="A43" s="1">
         <v>14</v>
       </c>
-      <c r="B43" t="s">
-        <v>6</v>
+      <c r="B43">
+        <v>1</v>
       </c>
       <c r="C43">
         <v>150</v>
@@ -1257,8 +1620,8 @@
       <c r="A44" s="1">
         <v>14</v>
       </c>
-      <c r="B44" t="s">
-        <v>6</v>
+      <c r="B44">
+        <v>1</v>
       </c>
       <c r="C44">
         <v>175</v>
@@ -1277,8 +1640,8 @@
       <c r="A45" s="1">
         <v>14</v>
       </c>
-      <c r="B45" t="s">
-        <v>6</v>
+      <c r="B45">
+        <v>1</v>
       </c>
       <c r="C45">
         <v>153</v>
@@ -1297,8 +1660,8 @@
       <c r="A46" s="1">
         <v>14</v>
       </c>
-      <c r="B46" t="s">
-        <v>6</v>
+      <c r="B46">
+        <v>1</v>
       </c>
       <c r="C46">
         <v>150</v>
@@ -1317,8 +1680,8 @@
       <c r="A47" s="1">
         <v>14</v>
       </c>
-      <c r="B47" t="s">
-        <v>6</v>
+      <c r="B47">
+        <v>1</v>
       </c>
       <c r="C47">
         <v>150</v>
@@ -1337,8 +1700,8 @@
       <c r="A48" s="1">
         <v>14</v>
       </c>
-      <c r="B48" t="s">
-        <v>6</v>
+      <c r="B48">
+        <v>1</v>
       </c>
       <c r="C48">
         <v>137</v>
@@ -1357,8 +1720,8 @@
       <c r="A49" s="1">
         <v>14</v>
       </c>
-      <c r="B49" t="s">
-        <v>6</v>
+      <c r="B49">
+        <v>1</v>
       </c>
       <c r="C49">
         <v>150</v>
@@ -1377,8 +1740,8 @@
       <c r="A50" s="1">
         <v>14</v>
       </c>
-      <c r="B50" t="s">
-        <v>6</v>
+      <c r="B50">
+        <v>1</v>
       </c>
       <c r="C50">
         <v>150</v>
@@ -1397,8 +1760,8 @@
       <c r="A51" s="1">
         <v>14</v>
       </c>
-      <c r="B51" t="s">
-        <v>6</v>
+      <c r="B51">
+        <v>1</v>
       </c>
       <c r="C51">
         <v>140</v>
@@ -1417,8 +1780,8 @@
       <c r="A52" s="1">
         <v>14</v>
       </c>
-      <c r="B52" t="s">
-        <v>6</v>
+      <c r="B52">
+        <v>1</v>
       </c>
       <c r="C52">
         <v>150</v>
@@ -1437,8 +1800,8 @@
       <c r="A53" s="1">
         <v>14</v>
       </c>
-      <c r="B53" t="s">
-        <v>6</v>
+      <c r="B53">
+        <v>1</v>
       </c>
       <c r="C53">
         <v>148</v>
@@ -1457,8 +1820,8 @@
       <c r="A54" s="1">
         <v>14.5</v>
       </c>
-      <c r="B54" t="s">
-        <v>6</v>
+      <c r="B54">
+        <v>1</v>
       </c>
       <c r="C54">
         <v>152</v>
@@ -1477,8 +1840,8 @@
       <c r="A55" s="1">
         <v>15</v>
       </c>
-      <c r="B55" t="s">
-        <v>6</v>
+      <c r="B55">
+        <v>1</v>
       </c>
       <c r="C55">
         <v>165</v>
@@ -1497,8 +1860,8 @@
       <c r="A56" s="1">
         <v>15</v>
       </c>
-      <c r="B56" t="s">
-        <v>6</v>
+      <c r="B56">
+        <v>1</v>
       </c>
       <c r="C56">
         <v>198</v>
@@ -1517,8 +1880,8 @@
       <c r="A57" s="1">
         <v>15</v>
       </c>
-      <c r="B57" t="s">
-        <v>6</v>
+      <c r="B57">
+        <v>1</v>
       </c>
       <c r="C57">
         <v>190</v>
@@ -1537,8 +1900,8 @@
       <c r="A58" s="1">
         <v>15</v>
       </c>
-      <c r="B58" t="s">
-        <v>6</v>
+      <c r="B58">
+        <v>1</v>
       </c>
       <c r="C58">
         <v>170</v>
@@ -1557,8 +1920,8 @@
       <c r="A59" s="1">
         <v>15</v>
       </c>
-      <c r="B59" t="s">
-        <v>6</v>
+      <c r="B59">
+        <v>1</v>
       </c>
       <c r="C59">
         <v>150</v>
@@ -1577,8 +1940,8 @@
       <c r="A60" s="1">
         <v>15</v>
       </c>
-      <c r="B60" t="s">
-        <v>6</v>
+      <c r="B60">
+        <v>1</v>
       </c>
       <c r="C60">
         <v>150</v>
@@ -1597,8 +1960,8 @@
       <c r="A61" s="1">
         <v>15</v>
       </c>
-      <c r="B61" t="s">
-        <v>6</v>
+      <c r="B61">
+        <v>1</v>
       </c>
       <c r="C61">
         <v>150</v>
@@ -1617,8 +1980,8 @@
       <c r="A62" s="1">
         <v>15</v>
       </c>
-      <c r="B62" t="s">
-        <v>6</v>
+      <c r="B62">
+        <v>1</v>
       </c>
       <c r="C62">
         <v>150</v>
@@ -1637,8 +2000,8 @@
       <c r="A63" s="1">
         <v>15</v>
       </c>
-      <c r="B63" t="s">
-        <v>6</v>
+      <c r="B63">
+        <v>1</v>
       </c>
       <c r="C63">
         <v>145</v>
@@ -1657,8 +2020,8 @@
       <c r="A64" s="1">
         <v>15</v>
       </c>
-      <c r="B64" t="s">
-        <v>6</v>
+      <c r="B64">
+        <v>1</v>
       </c>
       <c r="C64">
         <v>150</v>
@@ -1677,8 +2040,8 @@
       <c r="A65" s="1">
         <v>15</v>
       </c>
-      <c r="B65" t="s">
-        <v>7</v>
+      <c r="B65">
+        <v>2</v>
       </c>
       <c r="C65">
         <v>100</v>
@@ -1697,8 +2060,8 @@
       <c r="A66" s="1">
         <v>15</v>
       </c>
-      <c r="B66" t="s">
-        <v>7</v>
+      <c r="B66">
+        <v>2</v>
       </c>
       <c r="C66">
         <v>72</v>
@@ -1717,8 +2080,8 @@
       <c r="A67" s="1">
         <v>15</v>
       </c>
-      <c r="B67" t="s">
-        <v>7</v>
+      <c r="B67">
+        <v>2</v>
       </c>
       <c r="C67">
         <v>72</v>
@@ -1737,8 +2100,8 @@
       <c r="A68" s="1">
         <v>15</v>
       </c>
-      <c r="B68" t="s">
-        <v>6</v>
+      <c r="B68">
+        <v>1</v>
       </c>
       <c r="C68">
         <v>145</v>
@@ -1757,8 +2120,8 @@
       <c r="A69" s="1">
         <v>15</v>
       </c>
-      <c r="B69" t="s">
-        <v>7</v>
+      <c r="B69">
+        <v>2</v>
       </c>
       <c r="C69">
         <v>110</v>
@@ -1777,8 +2140,8 @@
       <c r="A70" s="1">
         <v>15</v>
       </c>
-      <c r="B70" t="s">
-        <v>6</v>
+      <c r="B70">
+        <v>1</v>
       </c>
       <c r="C70">
         <v>130</v>
@@ -1797,8 +2160,8 @@
       <c r="A71" s="1">
         <v>15.5</v>
       </c>
-      <c r="B71" t="s">
-        <v>6</v>
+      <c r="B71">
+        <v>1</v>
       </c>
       <c r="C71">
         <v>120</v>
@@ -1817,8 +2180,8 @@
       <c r="A72" s="1">
         <v>15.5</v>
       </c>
-      <c r="B72" t="s">
-        <v>6</v>
+      <c r="B72">
+        <v>1</v>
       </c>
       <c r="C72">
         <v>145</v>
@@ -1837,8 +2200,8 @@
       <c r="A73" s="1">
         <v>15.5</v>
       </c>
-      <c r="B73" t="s">
-        <v>6</v>
+      <c r="B73">
+        <v>1</v>
       </c>
       <c r="C73">
         <v>170</v>
@@ -1857,8 +2220,8 @@
       <c r="A74" s="1">
         <v>15.5</v>
       </c>
-      <c r="B74" t="s">
-        <v>6</v>
+      <c r="B74">
+        <v>1</v>
       </c>
       <c r="C74">
         <v>190</v>
@@ -1877,8 +2240,8 @@
       <c r="A75" s="1">
         <v>15.5</v>
       </c>
-      <c r="B75" t="s">
-        <v>6</v>
+      <c r="B75">
+        <v>1</v>
       </c>
       <c r="C75">
         <v>142</v>
@@ -1897,8 +2260,8 @@
       <c r="A76" s="1">
         <v>16</v>
       </c>
-      <c r="B76" t="s">
-        <v>6</v>
+      <c r="B76">
+        <v>1</v>
       </c>
       <c r="C76">
         <v>150</v>
@@ -1917,8 +2280,8 @@
       <c r="A77" s="1">
         <v>16</v>
       </c>
-      <c r="B77" t="s">
-        <v>7</v>
+      <c r="B77">
+        <v>2</v>
       </c>
       <c r="C77">
         <v>105</v>
@@ -1937,8 +2300,8 @@
       <c r="A78" s="1">
         <v>16</v>
       </c>
-      <c r="B78" t="s">
-        <v>7</v>
+      <c r="B78">
+        <v>2</v>
       </c>
       <c r="C78">
         <v>100</v>
@@ -1957,8 +2320,8 @@
       <c r="A79" s="1">
         <v>16</v>
       </c>
-      <c r="B79" t="s">
-        <v>6</v>
+      <c r="B79">
+        <v>1</v>
       </c>
       <c r="C79">
         <v>230</v>
@@ -1977,8 +2340,8 @@
       <c r="A80" s="1">
         <v>16</v>
       </c>
-      <c r="B80" t="s">
-        <v>7</v>
+      <c r="B80">
+        <v>2</v>
       </c>
       <c r="C80">
         <v>100</v>
@@ -1997,8 +2360,8 @@
       <c r="A81" s="1">
         <v>16</v>
       </c>
-      <c r="B81" t="s">
-        <v>7</v>
+      <c r="B81">
+        <v>2</v>
       </c>
       <c r="C81">
         <v>110</v>
@@ -2017,8 +2380,8 @@
       <c r="A82" s="1">
         <v>16</v>
       </c>
-      <c r="B82" t="s">
-        <v>6</v>
+      <c r="B82">
+        <v>1</v>
       </c>
       <c r="C82">
         <v>140</v>
@@ -2037,8 +2400,8 @@
       <c r="A83" s="1">
         <v>16</v>
       </c>
-      <c r="B83" t="s">
-        <v>6</v>
+      <c r="B83">
+        <v>1</v>
       </c>
       <c r="C83">
         <v>170</v>
@@ -2057,8 +2420,8 @@
       <c r="A84" s="1">
         <v>16</v>
       </c>
-      <c r="B84" t="s">
-        <v>6</v>
+      <c r="B84">
+        <v>1</v>
       </c>
       <c r="C84">
         <v>150</v>
@@ -2077,8 +2440,8 @@
       <c r="A85" s="1">
         <v>16</v>
       </c>
-      <c r="B85" t="s">
-        <v>7</v>
+      <c r="B85">
+        <v>2</v>
       </c>
       <c r="C85">
         <v>105</v>
@@ -2097,8 +2460,8 @@
       <c r="A86" s="1">
         <v>16</v>
       </c>
-      <c r="B86" t="s">
-        <v>6</v>
+      <c r="B86">
+        <v>1</v>
       </c>
       <c r="C86">
         <v>150</v>
@@ -2117,8 +2480,8 @@
       <c r="A87" s="1">
         <v>16</v>
       </c>
-      <c r="B87" t="s">
-        <v>6</v>
+      <c r="B87">
+        <v>1</v>
       </c>
       <c r="C87">
         <v>180</v>
@@ -2137,8 +2500,8 @@
       <c r="A88" s="1">
         <v>16</v>
       </c>
-      <c r="B88" t="s">
-        <v>6</v>
+      <c r="B88">
+        <v>1</v>
       </c>
       <c r="C88">
         <v>149</v>
@@ -2157,8 +2520,8 @@
       <c r="A89" s="1">
         <v>16.2</v>
       </c>
-      <c r="B89" t="s">
-        <v>7</v>
+      <c r="B89">
+        <v>2</v>
       </c>
       <c r="C89">
         <v>133</v>
@@ -2177,8 +2540,8 @@
       <c r="A90" s="1">
         <v>16.5</v>
       </c>
-      <c r="B90" t="s">
-        <v>7</v>
+      <c r="B90">
+        <v>2</v>
       </c>
       <c r="C90">
         <v>120</v>
@@ -2197,8 +2560,8 @@
       <c r="A91" s="1">
         <v>16.5</v>
       </c>
-      <c r="B91" t="s">
-        <v>6</v>
+      <c r="B91">
+        <v>1</v>
       </c>
       <c r="C91">
         <v>180</v>
@@ -2217,8 +2580,8 @@
       <c r="A92" s="1">
         <v>16.5</v>
       </c>
-      <c r="B92" t="s">
-        <v>6</v>
+      <c r="B92">
+        <v>1</v>
       </c>
       <c r="C92">
         <v>138</v>
@@ -2237,8 +2600,8 @@
       <c r="A93" s="1">
         <v>16.899999999999999</v>
       </c>
-      <c r="B93" t="s">
-        <v>6</v>
+      <c r="B93">
+        <v>1</v>
       </c>
       <c r="C93">
         <v>155</v>
@@ -2257,8 +2620,8 @@
       <c r="A94" s="1">
         <v>17</v>
       </c>
-      <c r="B94" t="s">
-        <v>6</v>
+      <c r="B94">
+        <v>1</v>
       </c>
       <c r="C94">
         <v>140</v>
@@ -2277,8 +2640,8 @@
       <c r="A95" s="1">
         <v>17</v>
       </c>
-      <c r="B95" t="s">
-        <v>7</v>
+      <c r="B95">
+        <v>2</v>
       </c>
       <c r="C95">
         <v>100</v>
@@ -2297,8 +2660,8 @@
       <c r="A96" s="1">
         <v>17</v>
       </c>
-      <c r="B96" t="s">
-        <v>6</v>
+      <c r="B96">
+        <v>1</v>
       </c>
       <c r="C96">
         <v>150</v>
@@ -2317,8 +2680,8 @@
       <c r="A97" s="1">
         <v>17</v>
       </c>
-      <c r="B97" t="s">
-        <v>7</v>
+      <c r="B97">
+        <v>2</v>
       </c>
       <c r="C97">
         <v>110</v>
@@ -2337,8 +2700,8 @@
       <c r="A98" s="1">
         <v>17</v>
       </c>
-      <c r="B98" t="s">
-        <v>6</v>
+      <c r="B98">
+        <v>1</v>
       </c>
       <c r="C98">
         <v>110</v>
@@ -2357,8 +2720,8 @@
       <c r="A99" s="1">
         <v>17</v>
       </c>
-      <c r="B99" t="s">
-        <v>7</v>
+      <c r="B99">
+        <v>2</v>
       </c>
       <c r="C99">
         <v>125</v>
@@ -2377,8 +2740,8 @@
       <c r="A100" s="1">
         <v>17</v>
       </c>
-      <c r="B100" t="s">
-        <v>6</v>
+      <c r="B100">
+        <v>1</v>
       </c>
       <c r="C100">
         <v>130</v>
@@ -2397,8 +2760,8 @@
       <c r="A101" s="1">
         <v>17.5</v>
       </c>
-      <c r="B101" t="s">
-        <v>6</v>
+      <c r="B101">
+        <v>1</v>
       </c>
       <c r="C101">
         <v>140</v>
@@ -2417,8 +2780,8 @@
       <c r="A102" s="1">
         <v>17.5</v>
       </c>
-      <c r="B102" t="s">
-        <v>7</v>
+      <c r="B102">
+        <v>2</v>
       </c>
       <c r="C102">
         <v>95</v>
@@ -2437,8 +2800,8 @@
       <c r="A103" s="1">
         <v>17.5</v>
       </c>
-      <c r="B103" t="s">
-        <v>6</v>
+      <c r="B103">
+        <v>1</v>
       </c>
       <c r="C103">
         <v>145</v>
@@ -2457,8 +2820,8 @@
       <c r="A104" s="1">
         <v>17.5</v>
       </c>
-      <c r="B104" t="s">
-        <v>7</v>
+      <c r="B104">
+        <v>2</v>
       </c>
       <c r="C104">
         <v>110</v>
@@ -2477,8 +2840,8 @@
       <c r="A105" s="1">
         <v>17.5</v>
       </c>
-      <c r="B105" t="s">
-        <v>6</v>
+      <c r="B105">
+        <v>1</v>
       </c>
       <c r="C105">
         <v>140</v>
@@ -2497,8 +2860,8 @@
       <c r="A106" s="1">
         <v>17.600000000000001</v>
       </c>
-      <c r="B106" t="s">
-        <v>6</v>
+      <c r="B106">
+        <v>1</v>
       </c>
       <c r="C106">
         <v>129</v>
@@ -2517,8 +2880,8 @@
       <c r="A107" s="1">
         <v>17.600000000000001</v>
       </c>
-      <c r="B107" t="s">
-        <v>7</v>
+      <c r="B107">
+        <v>2</v>
       </c>
       <c r="C107">
         <v>85</v>
@@ -2537,8 +2900,8 @@
       <c r="A108" s="1">
         <v>17.7</v>
       </c>
-      <c r="B108" t="s">
-        <v>7</v>
+      <c r="B108">
+        <v>2</v>
       </c>
       <c r="C108">
         <v>165</v>
@@ -2557,8 +2920,8 @@
       <c r="A109" s="1">
         <v>18</v>
       </c>
-      <c r="B109" t="s">
-        <v>6</v>
+      <c r="B109">
+        <v>1</v>
       </c>
       <c r="C109">
         <v>130</v>
@@ -2577,8 +2940,8 @@
       <c r="A110" s="1">
         <v>18</v>
       </c>
-      <c r="B110" t="s">
-        <v>6</v>
+      <c r="B110">
+        <v>1</v>
       </c>
       <c r="C110">
         <v>150</v>
@@ -2597,8 +2960,8 @@
       <c r="A111" s="1">
         <v>18</v>
       </c>
-      <c r="B111" t="s">
-        <v>7</v>
+      <c r="B111">
+        <v>2</v>
       </c>
       <c r="C111">
         <v>97</v>
@@ -2617,8 +2980,8 @@
       <c r="A112" s="1">
         <v>18</v>
       </c>
-      <c r="B112" t="s">
-        <v>7</v>
+      <c r="B112">
+        <v>2</v>
       </c>
       <c r="C112">
         <v>100</v>
@@ -2637,8 +3000,8 @@
       <c r="A113" s="1">
         <v>18</v>
       </c>
-      <c r="B113" t="s">
-        <v>7</v>
+      <c r="B113">
+        <v>2</v>
       </c>
       <c r="C113">
         <v>110</v>
@@ -2657,8 +3020,8 @@
       <c r="A114" s="1">
         <v>18</v>
       </c>
-      <c r="B114" t="s">
-        <v>7</v>
+      <c r="B114">
+        <v>2</v>
       </c>
       <c r="C114">
         <v>88</v>
@@ -2677,8 +3040,8 @@
       <c r="A115" s="1">
         <v>18</v>
       </c>
-      <c r="B115" t="s">
-        <v>8</v>
+      <c r="B115">
+        <v>3</v>
       </c>
       <c r="C115">
         <v>112</v>
@@ -2697,8 +3060,8 @@
       <c r="A116" s="1">
         <v>18</v>
       </c>
-      <c r="B116" t="s">
-        <v>7</v>
+      <c r="B116">
+        <v>2</v>
       </c>
       <c r="C116">
         <v>105</v>
@@ -2717,8 +3080,8 @@
       <c r="A117" s="1">
         <v>18</v>
       </c>
-      <c r="B117" t="s">
-        <v>7</v>
+      <c r="B117">
+        <v>2</v>
       </c>
       <c r="C117">
         <v>100</v>
@@ -2737,8 +3100,8 @@
       <c r="A118" s="1">
         <v>18</v>
       </c>
-      <c r="B118" t="s">
-        <v>7</v>
+      <c r="B118">
+        <v>2</v>
       </c>
       <c r="C118">
         <v>88</v>
@@ -2757,8 +3120,8 @@
       <c r="A119" s="1">
         <v>18</v>
       </c>
-      <c r="B119" t="s">
-        <v>7</v>
+      <c r="B119">
+        <v>2</v>
       </c>
       <c r="C119">
         <v>100</v>
@@ -2777,8 +3140,8 @@
       <c r="A120" s="1">
         <v>18</v>
       </c>
-      <c r="B120" t="s">
-        <v>9</v>
+      <c r="B120">
+        <v>4</v>
       </c>
       <c r="C120">
         <v>90</v>
@@ -2797,8 +3160,8 @@
       <c r="A121" s="1">
         <v>18</v>
       </c>
-      <c r="B121" t="s">
-        <v>7</v>
+      <c r="B121">
+        <v>2</v>
       </c>
       <c r="C121">
         <v>105</v>
@@ -2817,8 +3180,8 @@
       <c r="A122" s="1">
         <v>18</v>
       </c>
-      <c r="B122" t="s">
-        <v>7</v>
+      <c r="B122">
+        <v>2</v>
       </c>
       <c r="C122">
         <v>105</v>
@@ -2837,8 +3200,8 @@
       <c r="A123" s="1">
         <v>18</v>
       </c>
-      <c r="B123" t="s">
-        <v>7</v>
+      <c r="B123">
+        <v>2</v>
       </c>
       <c r="C123">
         <v>95</v>
@@ -2857,8 +3220,8 @@
       <c r="A124" s="1">
         <v>18</v>
       </c>
-      <c r="B124" t="s">
-        <v>7</v>
+      <c r="B124">
+        <v>2</v>
       </c>
       <c r="C124">
         <v>97</v>
@@ -2877,8 +3240,8 @@
       <c r="A125" s="1">
         <v>18</v>
       </c>
-      <c r="B125" t="s">
-        <v>7</v>
+      <c r="B125">
+        <v>2</v>
       </c>
       <c r="C125">
         <v>78</v>
@@ -2897,8 +3260,8 @@
       <c r="A126" s="1">
         <v>18.100000000000001</v>
       </c>
-      <c r="B126" t="s">
-        <v>7</v>
+      <c r="B126">
+        <v>2</v>
       </c>
       <c r="C126">
         <v>120</v>
@@ -2917,8 +3280,8 @@
       <c r="A127" s="1">
         <v>18.100000000000001</v>
       </c>
-      <c r="B127" t="s">
-        <v>6</v>
+      <c r="B127">
+        <v>1</v>
       </c>
       <c r="C127">
         <v>139</v>
@@ -2937,8 +3300,8 @@
       <c r="A128" s="1">
         <v>18.2</v>
       </c>
-      <c r="B128" t="s">
-        <v>6</v>
+      <c r="B128">
+        <v>1</v>
       </c>
       <c r="C128">
         <v>135</v>
@@ -2957,8 +3320,8 @@
       <c r="A129" s="1">
         <v>18.5</v>
       </c>
-      <c r="B129" t="s">
-        <v>7</v>
+      <c r="B129">
+        <v>2</v>
       </c>
       <c r="C129">
         <v>110</v>
@@ -2977,8 +3340,8 @@
       <c r="A130" s="1">
         <v>18.5</v>
       </c>
-      <c r="B130" t="s">
-        <v>7</v>
+      <c r="B130">
+        <v>2</v>
       </c>
       <c r="C130">
         <v>98</v>
@@ -2997,8 +3360,8 @@
       <c r="A131" s="1">
         <v>18.5</v>
       </c>
-      <c r="B131" t="s">
-        <v>6</v>
+      <c r="B131">
+        <v>1</v>
       </c>
       <c r="C131">
         <v>150</v>
@@ -3017,8 +3380,8 @@
       <c r="A132" s="1">
         <v>18.600000000000001</v>
       </c>
-      <c r="B132" t="s">
-        <v>7</v>
+      <c r="B132">
+        <v>2</v>
       </c>
       <c r="C132">
         <v>110</v>
@@ -3037,8 +3400,8 @@
       <c r="A133" s="1">
         <v>19</v>
       </c>
-      <c r="B133" t="s">
-        <v>7</v>
+      <c r="B133">
+        <v>2</v>
       </c>
       <c r="C133">
         <v>100</v>
@@ -3057,8 +3420,8 @@
       <c r="A134" s="1">
         <v>19</v>
       </c>
-      <c r="B134" t="s">
-        <v>7</v>
+      <c r="B134">
+        <v>2</v>
       </c>
       <c r="C134">
         <v>88</v>
@@ -3077,8 +3440,8 @@
       <c r="A135" s="1">
         <v>19</v>
       </c>
-      <c r="B135" t="s">
-        <v>7</v>
+      <c r="B135">
+        <v>2</v>
       </c>
       <c r="C135">
         <v>100</v>
@@ -3097,8 +3460,8 @@
       <c r="A136" s="1">
         <v>19</v>
       </c>
-      <c r="B136" t="s">
-        <v>9</v>
+      <c r="B136">
+        <v>4</v>
       </c>
       <c r="C136">
         <v>97</v>
@@ -3117,8 +3480,8 @@
       <c r="A137" s="1">
         <v>19</v>
       </c>
-      <c r="B137" t="s">
-        <v>8</v>
+      <c r="B137">
+        <v>3</v>
       </c>
       <c r="C137">
         <v>85</v>
@@ -3137,8 +3500,8 @@
       <c r="A138" s="1">
         <v>19</v>
       </c>
-      <c r="B138" t="s">
-        <v>8</v>
+      <c r="B138">
+        <v>3</v>
       </c>
       <c r="C138">
         <v>112</v>
@@ -3157,8 +3520,8 @@
       <c r="A139" s="1">
         <v>19</v>
       </c>
-      <c r="B139" t="s">
-        <v>7</v>
+      <c r="B139">
+        <v>2</v>
       </c>
       <c r="C139">
         <v>100</v>
@@ -3177,8 +3540,8 @@
       <c r="A140" s="1">
         <v>19</v>
       </c>
-      <c r="B140" t="s">
-        <v>7</v>
+      <c r="B140">
+        <v>2</v>
       </c>
       <c r="C140">
         <v>95</v>
@@ -3197,8 +3560,8 @@
       <c r="A141" s="1">
         <v>19</v>
       </c>
-      <c r="B141" t="s">
-        <v>7</v>
+      <c r="B141">
+        <v>2</v>
       </c>
       <c r="C141">
         <v>90</v>
@@ -3217,8 +3580,8 @@
       <c r="A142" s="1">
         <v>19</v>
       </c>
-      <c r="B142" t="s">
-        <v>8</v>
+      <c r="B142">
+        <v>3</v>
       </c>
       <c r="C142">
         <v>88</v>
@@ -3237,8 +3600,8 @@
       <c r="A143" s="1">
         <v>19</v>
       </c>
-      <c r="B143" t="s">
-        <v>7</v>
+      <c r="B143">
+        <v>2</v>
       </c>
       <c r="C143">
         <v>108</v>
@@ -3257,8 +3620,8 @@
       <c r="A144" s="1">
         <v>19</v>
       </c>
-      <c r="B144" t="s">
-        <v>7</v>
+      <c r="B144">
+        <v>2</v>
       </c>
       <c r="C144">
         <v>100</v>
@@ -3277,8 +3640,8 @@
       <c r="A145" s="1">
         <v>19.100000000000001</v>
       </c>
-      <c r="B145" t="s">
-        <v>7</v>
+      <c r="B145">
+        <v>2</v>
       </c>
       <c r="C145">
         <v>90</v>
@@ -3297,8 +3660,8 @@
       <c r="A146" s="1">
         <v>19.2</v>
       </c>
-      <c r="B146" t="s">
-        <v>7</v>
+      <c r="B146">
+        <v>2</v>
       </c>
       <c r="C146">
         <v>105</v>
@@ -3317,8 +3680,8 @@
       <c r="A147" s="1">
         <v>19.2</v>
       </c>
-      <c r="B147" t="s">
-        <v>6</v>
+      <c r="B147">
+        <v>1</v>
       </c>
       <c r="C147">
         <v>145</v>
@@ -3337,8 +3700,8 @@
       <c r="A148" s="1">
         <v>19.2</v>
       </c>
-      <c r="B148" t="s">
-        <v>6</v>
+      <c r="B148">
+        <v>1</v>
       </c>
       <c r="C148">
         <v>125</v>
@@ -3357,8 +3720,8 @@
       <c r="A149" s="1">
         <v>19.399999999999999</v>
       </c>
-      <c r="B149" t="s">
-        <v>6</v>
+      <c r="B149">
+        <v>1</v>
       </c>
       <c r="C149">
         <v>140</v>
@@ -3377,8 +3740,8 @@
       <c r="A150" s="1">
         <v>19.399999999999999</v>
       </c>
-      <c r="B150" t="s">
-        <v>7</v>
+      <c r="B150">
+        <v>2</v>
       </c>
       <c r="C150">
         <v>90</v>
@@ -3397,8 +3760,8 @@
       <c r="A151" s="1">
         <v>19.8</v>
       </c>
-      <c r="B151" t="s">
-        <v>7</v>
+      <c r="B151">
+        <v>2</v>
       </c>
       <c r="C151">
         <v>85</v>
@@ -3417,8 +3780,8 @@
       <c r="A152" s="1">
         <v>19.899999999999999</v>
       </c>
-      <c r="B152" t="s">
-        <v>6</v>
+      <c r="B152">
+        <v>1</v>
       </c>
       <c r="C152">
         <v>110</v>
@@ -3437,8 +3800,8 @@
       <c r="A153" s="1">
         <v>20</v>
       </c>
-      <c r="B153" t="s">
-        <v>8</v>
+      <c r="B153">
+        <v>3</v>
       </c>
       <c r="C153">
         <v>90</v>
@@ -3457,8 +3820,8 @@
       <c r="A154" s="1">
         <v>20</v>
       </c>
-      <c r="B154" t="s">
-        <v>8</v>
+      <c r="B154">
+        <v>3</v>
       </c>
       <c r="C154">
         <v>88</v>
@@ -3477,8 +3840,8 @@
       <c r="A155" s="1">
         <v>20</v>
       </c>
-      <c r="B155" t="s">
-        <v>8</v>
+      <c r="B155">
+        <v>3</v>
       </c>
       <c r="C155">
         <v>91</v>
@@ -3497,8 +3860,8 @@
       <c r="A156" s="1">
         <v>20</v>
       </c>
-      <c r="B156" t="s">
-        <v>7</v>
+      <c r="B156">
+        <v>2</v>
       </c>
       <c r="C156">
         <v>122</v>
@@ -3517,8 +3880,8 @@
       <c r="A157" s="1">
         <v>20</v>
       </c>
-      <c r="B157" t="s">
-        <v>7</v>
+      <c r="B157">
+        <v>2</v>
       </c>
       <c r="C157">
         <v>95</v>
@@ -3537,8 +3900,8 @@
       <c r="A158" s="1">
         <v>20</v>
       </c>
-      <c r="B158" t="s">
-        <v>6</v>
+      <c r="B158">
+        <v>1</v>
       </c>
       <c r="C158">
         <v>110</v>
@@ -3557,8 +3920,8 @@
       <c r="A159" s="1">
         <v>20</v>
       </c>
-      <c r="B159" t="s">
-        <v>7</v>
+      <c r="B159">
+        <v>2</v>
       </c>
       <c r="C159">
         <v>100</v>
@@ -3577,8 +3940,8 @@
       <c r="A160" s="1">
         <v>20</v>
       </c>
-      <c r="B160" t="s">
-        <v>7</v>
+      <c r="B160">
+        <v>2</v>
       </c>
       <c r="C160">
         <v>100</v>
@@ -3597,8 +3960,8 @@
       <c r="A161" s="1">
         <v>20</v>
       </c>
-      <c r="B161" t="s">
-        <v>8</v>
+      <c r="B161">
+        <v>3</v>
       </c>
       <c r="C161">
         <v>102</v>
@@ -3617,8 +3980,8 @@
       <c r="A162" s="1">
         <v>20.2</v>
       </c>
-      <c r="B162" t="s">
-        <v>6</v>
+      <c r="B162">
+        <v>1</v>
       </c>
       <c r="C162">
         <v>139</v>
@@ -3637,8 +4000,8 @@
       <c r="A163" s="1">
         <v>20.2</v>
       </c>
-      <c r="B163" t="s">
-        <v>7</v>
+      <c r="B163">
+        <v>2</v>
       </c>
       <c r="C163">
         <v>85</v>
@@ -3657,8 +4020,8 @@
       <c r="A164" s="1">
         <v>20.2</v>
       </c>
-      <c r="B164" t="s">
-        <v>7</v>
+      <c r="B164">
+        <v>2</v>
       </c>
       <c r="C164">
         <v>90</v>
@@ -3677,8 +4040,8 @@
       <c r="A165" s="1">
         <v>20.2</v>
       </c>
-      <c r="B165" t="s">
-        <v>7</v>
+      <c r="B165">
+        <v>2</v>
       </c>
       <c r="C165">
         <v>88</v>
@@ -3697,8 +4060,8 @@
       <c r="A166" s="1">
         <v>20.3</v>
       </c>
-      <c r="B166" t="s">
-        <v>10</v>
+      <c r="B166">
+        <v>5</v>
       </c>
       <c r="C166">
         <v>103</v>
@@ -3717,8 +4080,8 @@
       <c r="A167" s="1">
         <v>20.5</v>
       </c>
-      <c r="B167" t="s">
-        <v>7</v>
+      <c r="B167">
+        <v>2</v>
       </c>
       <c r="C167">
         <v>105</v>
@@ -3737,8 +4100,8 @@
       <c r="A168" s="1">
         <v>20.5</v>
       </c>
-      <c r="B168" t="s">
-        <v>7</v>
+      <c r="B168">
+        <v>2</v>
       </c>
       <c r="C168">
         <v>95</v>
@@ -3757,8 +4120,8 @@
       <c r="A169" s="1">
         <v>20.5</v>
       </c>
-      <c r="B169" t="s">
-        <v>7</v>
+      <c r="B169">
+        <v>2</v>
       </c>
       <c r="C169">
         <v>100</v>
@@ -3777,8 +4140,8 @@
       <c r="A170" s="1">
         <v>20.6</v>
       </c>
-      <c r="B170" t="s">
-        <v>7</v>
+      <c r="B170">
+        <v>2</v>
       </c>
       <c r="C170">
         <v>105</v>
@@ -3797,8 +4160,8 @@
       <c r="A171" s="1">
         <v>20.6</v>
       </c>
-      <c r="B171" t="s">
-        <v>7</v>
+      <c r="B171">
+        <v>2</v>
       </c>
       <c r="C171">
         <v>110</v>
@@ -3817,8 +4180,8 @@
       <c r="A172" s="1">
         <v>20.8</v>
       </c>
-      <c r="B172" t="s">
-        <v>7</v>
+      <c r="B172">
+        <v>2</v>
       </c>
       <c r="C172">
         <v>85</v>
@@ -3837,8 +4200,8 @@
       <c r="A173" s="1">
         <v>21</v>
       </c>
-      <c r="B173" t="s">
-        <v>7</v>
+      <c r="B173">
+        <v>2</v>
       </c>
       <c r="C173">
         <v>85</v>
@@ -3857,8 +4220,8 @@
       <c r="A174" s="1">
         <v>21</v>
       </c>
-      <c r="B174" t="s">
-        <v>7</v>
+      <c r="B174">
+        <v>2</v>
       </c>
       <c r="C174">
         <v>90</v>
@@ -3877,8 +4240,8 @@
       <c r="A175" s="1">
         <v>21</v>
       </c>
-      <c r="B175" t="s">
-        <v>8</v>
+      <c r="B175">
+        <v>3</v>
       </c>
       <c r="C175">
         <v>86</v>
@@ -3897,8 +4260,8 @@
       <c r="A176" s="1">
         <v>21</v>
       </c>
-      <c r="B176" t="s">
-        <v>8</v>
+      <c r="B176">
+        <v>3</v>
       </c>
       <c r="C176">
         <v>87</v>
@@ -3917,8 +4280,8 @@
       <c r="A177" s="1">
         <v>21</v>
       </c>
-      <c r="B177" t="s">
-        <v>8</v>
+      <c r="B177">
+        <v>3</v>
       </c>
       <c r="C177">
         <v>72</v>
@@ -3937,8 +4300,8 @@
       <c r="A178" s="1">
         <v>21</v>
       </c>
-      <c r="B178" t="s">
-        <v>7</v>
+      <c r="B178">
+        <v>2</v>
       </c>
       <c r="C178">
         <v>107</v>
@@ -3957,8 +4320,8 @@
       <c r="A179" s="1">
         <v>21</v>
       </c>
-      <c r="B179" t="s">
-        <v>7</v>
+      <c r="B179">
+        <v>2</v>
       </c>
       <c r="C179">
         <v>110</v>
@@ -3977,8 +4340,8 @@
       <c r="A180" s="1">
         <v>21.1</v>
       </c>
-      <c r="B180" t="s">
-        <v>8</v>
+      <c r="B180">
+        <v>3</v>
       </c>
       <c r="C180">
         <v>95</v>
@@ -3997,8 +4360,8 @@
       <c r="A181" s="1">
         <v>21.5</v>
       </c>
-      <c r="B181" t="s">
-        <v>8</v>
+      <c r="B181">
+        <v>3</v>
       </c>
       <c r="C181">
         <v>110</v>
@@ -4017,8 +4380,8 @@
       <c r="A182" s="1">
         <v>21.5</v>
       </c>
-      <c r="B182" t="s">
-        <v>9</v>
+      <c r="B182">
+        <v>4</v>
       </c>
       <c r="C182">
         <v>110</v>
@@ -4037,8 +4400,8 @@
       <c r="A183" s="1">
         <v>21.5</v>
       </c>
-      <c r="B183" t="s">
-        <v>7</v>
+      <c r="B183">
+        <v>2</v>
       </c>
       <c r="C183">
         <v>115</v>
@@ -4057,8 +4420,8 @@
       <c r="A184" s="1">
         <v>21.6</v>
       </c>
-      <c r="B184" t="s">
-        <v>8</v>
+      <c r="B184">
+        <v>3</v>
       </c>
       <c r="C184">
         <v>115</v>
@@ -4077,8 +4440,8 @@
       <c r="A185" s="1">
         <v>22</v>
       </c>
-      <c r="B185" t="s">
-        <v>7</v>
+      <c r="B185">
+        <v>2</v>
       </c>
       <c r="C185">
         <v>95</v>
@@ -4097,8 +4460,8 @@
       <c r="A186" s="1">
         <v>22</v>
       </c>
-      <c r="B186" t="s">
-        <v>8</v>
+      <c r="B186">
+        <v>3</v>
       </c>
       <c r="C186">
         <v>72</v>
@@ -4117,8 +4480,8 @@
       <c r="A187" s="1">
         <v>22</v>
       </c>
-      <c r="B187" t="s">
-        <v>8</v>
+      <c r="B187">
+        <v>3</v>
       </c>
       <c r="C187">
         <v>76</v>
@@ -4137,8 +4500,8 @@
       <c r="A188" s="1">
         <v>22</v>
       </c>
-      <c r="B188" t="s">
-        <v>8</v>
+      <c r="B188">
+        <v>3</v>
       </c>
       <c r="C188">
         <v>86</v>
@@ -4157,8 +4520,8 @@
       <c r="A189" s="1">
         <v>22</v>
       </c>
-      <c r="B189" t="s">
-        <v>8</v>
+      <c r="B189">
+        <v>3</v>
       </c>
       <c r="C189">
         <v>94</v>
@@ -4177,8 +4540,8 @@
       <c r="A190" s="1">
         <v>22</v>
       </c>
-      <c r="B190" t="s">
-        <v>8</v>
+      <c r="B190">
+        <v>3</v>
       </c>
       <c r="C190">
         <v>98</v>
@@ -4197,8 +4560,8 @@
       <c r="A191" s="1">
         <v>22</v>
       </c>
-      <c r="B191" t="s">
-        <v>7</v>
+      <c r="B191">
+        <v>2</v>
       </c>
       <c r="C191">
         <v>100</v>
@@ -4217,8 +4580,8 @@
       <c r="A192" s="1">
         <v>22</v>
       </c>
-      <c r="B192" t="s">
-        <v>7</v>
+      <c r="B192">
+        <v>2</v>
       </c>
       <c r="C192">
         <v>105</v>
@@ -4237,8 +4600,8 @@
       <c r="A193" s="1">
         <v>22</v>
       </c>
-      <c r="B193" t="s">
-        <v>7</v>
+      <c r="B193">
+        <v>2</v>
       </c>
       <c r="C193">
         <v>97</v>
@@ -4257,8 +4620,8 @@
       <c r="A194" s="1">
         <v>22</v>
       </c>
-      <c r="B194" t="s">
-        <v>7</v>
+      <c r="B194">
+        <v>2</v>
       </c>
       <c r="C194">
         <v>112</v>
@@ -4277,8 +4640,8 @@
       <c r="A195" s="1">
         <v>22.3</v>
       </c>
-      <c r="B195" t="s">
-        <v>8</v>
+      <c r="B195">
+        <v>3</v>
       </c>
       <c r="C195">
         <v>88</v>
@@ -4297,8 +4660,8 @@
       <c r="A196" s="1">
         <v>22.4</v>
       </c>
-      <c r="B196" t="s">
-        <v>7</v>
+      <c r="B196">
+        <v>2</v>
       </c>
       <c r="C196">
         <v>110</v>
@@ -4317,8 +4680,8 @@
       <c r="A197" s="1">
         <v>22.5</v>
       </c>
-      <c r="B197" t="s">
-        <v>7</v>
+      <c r="B197">
+        <v>2</v>
       </c>
       <c r="C197">
         <v>90</v>
@@ -4337,8 +4700,8 @@
       <c r="A198" s="1">
         <v>23</v>
       </c>
-      <c r="B198" t="s">
-        <v>8</v>
+      <c r="B198">
+        <v>3</v>
       </c>
       <c r="C198">
         <v>86</v>
@@ -4357,8 +4720,8 @@
       <c r="A199" s="1">
         <v>23</v>
       </c>
-      <c r="B199" t="s">
-        <v>8</v>
+      <c r="B199">
+        <v>3</v>
       </c>
       <c r="C199">
         <v>54</v>
@@ -4377,8 +4740,8 @@
       <c r="A200" s="1">
         <v>23</v>
       </c>
-      <c r="B200" t="s">
-        <v>8</v>
+      <c r="B200">
+        <v>3</v>
       </c>
       <c r="C200">
         <v>97</v>
@@ -4397,8 +4760,8 @@
       <c r="A201" s="1">
         <v>23</v>
       </c>
-      <c r="B201" t="s">
-        <v>7</v>
+      <c r="B201">
+        <v>2</v>
       </c>
       <c r="C201">
         <v>95</v>
@@ -4417,8 +4780,8 @@
       <c r="A202" s="1">
         <v>23</v>
       </c>
-      <c r="B202" t="s">
-        <v>8</v>
+      <c r="B202">
+        <v>3</v>
       </c>
       <c r="C202">
         <v>83</v>
@@ -4437,8 +4800,8 @@
       <c r="A203" s="1">
         <v>23</v>
       </c>
-      <c r="B203" t="s">
-        <v>8</v>
+      <c r="B203">
+        <v>3</v>
       </c>
       <c r="C203">
         <v>78</v>
@@ -4457,8 +4820,8 @@
       <c r="A204" s="1">
         <v>23</v>
       </c>
-      <c r="B204" t="s">
-        <v>8</v>
+      <c r="B204">
+        <v>3</v>
       </c>
       <c r="C204">
         <v>95</v>
@@ -4477,8 +4840,8 @@
       <c r="A205" s="1">
         <v>23</v>
       </c>
-      <c r="B205" t="s">
-        <v>8</v>
+      <c r="B205">
+        <v>3</v>
       </c>
       <c r="C205">
         <v>88</v>
@@ -4497,8 +4860,8 @@
       <c r="A206" s="1">
         <v>23</v>
       </c>
-      <c r="B206" t="s">
-        <v>6</v>
+      <c r="B206">
+        <v>1</v>
       </c>
       <c r="C206">
         <v>125</v>
@@ -4517,8 +4880,8 @@
       <c r="A207" s="1">
         <v>23.2</v>
       </c>
-      <c r="B207" t="s">
-        <v>8</v>
+      <c r="B207">
+        <v>3</v>
       </c>
       <c r="C207">
         <v>105</v>
@@ -4537,8 +4900,8 @@
       <c r="A208" s="1">
         <v>23.5</v>
       </c>
-      <c r="B208" t="s">
-        <v>7</v>
+      <c r="B208">
+        <v>2</v>
       </c>
       <c r="C208">
         <v>110</v>
@@ -4557,8 +4920,8 @@
       <c r="A209" s="1">
         <v>23.7</v>
       </c>
-      <c r="B209" t="s">
-        <v>9</v>
+      <c r="B209">
+        <v>4</v>
       </c>
       <c r="C209">
         <v>100</v>
@@ -4577,8 +4940,8 @@
       <c r="A210" s="1">
         <v>23.8</v>
       </c>
-      <c r="B210" t="s">
-        <v>8</v>
+      <c r="B210">
+        <v>3</v>
       </c>
       <c r="C210">
         <v>85</v>
@@ -4597,8 +4960,8 @@
       <c r="A211" s="1">
         <v>23.9</v>
       </c>
-      <c r="B211" t="s">
-        <v>8</v>
+      <c r="B211">
+        <v>3</v>
       </c>
       <c r="C211">
         <v>97</v>
@@ -4617,8 +4980,8 @@
       <c r="A212" s="1">
         <v>23.9</v>
       </c>
-      <c r="B212" t="s">
-        <v>6</v>
+      <c r="B212">
+        <v>1</v>
       </c>
       <c r="C212">
         <v>90</v>
@@ -4637,8 +5000,8 @@
       <c r="A213" s="1">
         <v>24</v>
       </c>
-      <c r="B213" t="s">
-        <v>8</v>
+      <c r="B213">
+        <v>3</v>
       </c>
       <c r="C213">
         <v>95</v>
@@ -4657,8 +5020,8 @@
       <c r="A214" s="1">
         <v>24</v>
       </c>
-      <c r="B214" t="s">
-        <v>8</v>
+      <c r="B214">
+        <v>3</v>
       </c>
       <c r="C214">
         <v>90</v>
@@ -4677,8 +5040,8 @@
       <c r="A215" s="1">
         <v>24</v>
       </c>
-      <c r="B215" t="s">
-        <v>8</v>
+      <c r="B215">
+        <v>3</v>
       </c>
       <c r="C215">
         <v>95</v>
@@ -4697,8 +5060,8 @@
       <c r="A216" s="1">
         <v>24</v>
       </c>
-      <c r="B216" t="s">
-        <v>8</v>
+      <c r="B216">
+        <v>3</v>
       </c>
       <c r="C216">
         <v>75</v>
@@ -4717,8 +5080,8 @@
       <c r="A217" s="1">
         <v>24</v>
       </c>
-      <c r="B217" t="s">
-        <v>8</v>
+      <c r="B217">
+        <v>3</v>
       </c>
       <c r="C217">
         <v>110</v>
@@ -4737,8 +5100,8 @@
       <c r="A218" s="1">
         <v>24</v>
       </c>
-      <c r="B218" t="s">
-        <v>8</v>
+      <c r="B218">
+        <v>3</v>
       </c>
       <c r="C218">
         <v>75</v>
@@ -4757,8 +5120,8 @@
       <c r="A219" s="1">
         <v>24</v>
       </c>
-      <c r="B219" t="s">
-        <v>8</v>
+      <c r="B219">
+        <v>3</v>
       </c>
       <c r="C219">
         <v>97</v>
@@ -4777,8 +5140,8 @@
       <c r="A220" s="1">
         <v>24</v>
       </c>
-      <c r="B220" t="s">
-        <v>8</v>
+      <c r="B220">
+        <v>3</v>
       </c>
       <c r="C220">
         <v>96</v>
@@ -4797,8 +5160,8 @@
       <c r="A221" s="1">
         <v>24</v>
       </c>
-      <c r="B221" t="s">
-        <v>8</v>
+      <c r="B221">
+        <v>3</v>
       </c>
       <c r="C221">
         <v>97</v>
@@ -4817,8 +5180,8 @@
       <c r="A222" s="1">
         <v>24</v>
       </c>
-      <c r="B222" t="s">
-        <v>7</v>
+      <c r="B222">
+        <v>2</v>
       </c>
       <c r="C222">
         <v>81</v>
@@ -4837,8 +5200,8 @@
       <c r="A223" s="1">
         <v>24</v>
       </c>
-      <c r="B223" t="s">
-        <v>8</v>
+      <c r="B223">
+        <v>3</v>
       </c>
       <c r="C223">
         <v>92</v>
@@ -4857,8 +5220,8 @@
       <c r="A224" s="1">
         <v>24.2</v>
       </c>
-      <c r="B224" t="s">
-        <v>7</v>
+      <c r="B224">
+        <v>2</v>
       </c>
       <c r="C224">
         <v>120</v>
@@ -4877,8 +5240,8 @@
       <c r="A225" s="1">
         <v>24.3</v>
       </c>
-      <c r="B225" t="s">
-        <v>8</v>
+      <c r="B225">
+        <v>3</v>
       </c>
       <c r="C225">
         <v>90</v>
@@ -4897,8 +5260,8 @@
       <c r="A226" s="1">
         <v>24.5</v>
       </c>
-      <c r="B226" t="s">
-        <v>8</v>
+      <c r="B226">
+        <v>3</v>
       </c>
       <c r="C226">
         <v>60</v>
@@ -4917,8 +5280,8 @@
       <c r="A227" s="1">
         <v>24.5</v>
       </c>
-      <c r="B227" t="s">
-        <v>8</v>
+      <c r="B227">
+        <v>3</v>
       </c>
       <c r="C227">
         <v>88</v>
@@ -4937,8 +5300,8 @@
       <c r="A228" s="1">
         <v>25</v>
       </c>
-      <c r="B228" t="s">
-        <v>8</v>
+      <c r="B228">
+        <v>3</v>
       </c>
       <c r="C228">
         <v>87</v>
@@ -4957,8 +5320,8 @@
       <c r="A229" s="1">
         <v>25</v>
       </c>
-      <c r="B229" t="s">
-        <v>8</v>
+      <c r="B229">
+        <v>3</v>
       </c>
       <c r="C229">
         <v>95</v>
@@ -4977,8 +5340,8 @@
       <c r="A230" s="1">
         <v>25</v>
       </c>
-      <c r="B230" t="s">
-        <v>8</v>
+      <c r="B230">
+        <v>3</v>
       </c>
       <c r="C230">
         <v>95</v>
@@ -4997,8 +5360,8 @@
       <c r="A231" s="1">
         <v>25</v>
       </c>
-      <c r="B231" t="s">
-        <v>8</v>
+      <c r="B231">
+        <v>3</v>
       </c>
       <c r="C231">
         <v>80</v>
@@ -5017,8 +5380,8 @@
       <c r="A232" s="1">
         <v>25</v>
       </c>
-      <c r="B232" t="s">
-        <v>8</v>
+      <c r="B232">
+        <v>3</v>
       </c>
       <c r="C232">
         <v>75</v>
@@ -5037,8 +5400,8 @@
       <c r="A233" s="1">
         <v>25</v>
       </c>
-      <c r="B233" t="s">
-        <v>8</v>
+      <c r="B233">
+        <v>3</v>
       </c>
       <c r="C233">
         <v>71</v>
@@ -5057,8 +5420,8 @@
       <c r="A234" s="1">
         <v>25</v>
       </c>
-      <c r="B234" t="s">
-        <v>8</v>
+      <c r="B234">
+        <v>3</v>
       </c>
       <c r="C234">
         <v>115</v>
@@ -5077,8 +5440,8 @@
       <c r="A235" s="1">
         <v>25</v>
       </c>
-      <c r="B235" t="s">
-        <v>8</v>
+      <c r="B235">
+        <v>3</v>
       </c>
       <c r="C235">
         <v>81</v>
@@ -5097,8 +5460,8 @@
       <c r="A236" s="1">
         <v>25</v>
       </c>
-      <c r="B236" t="s">
-        <v>8</v>
+      <c r="B236">
+        <v>3</v>
       </c>
       <c r="C236">
         <v>92</v>
@@ -5117,8 +5480,8 @@
       <c r="A237" s="1">
         <v>25</v>
       </c>
-      <c r="B237" t="s">
-        <v>7</v>
+      <c r="B237">
+        <v>2</v>
       </c>
       <c r="C237">
         <v>110</v>
@@ -5137,8 +5500,8 @@
       <c r="A238" s="1">
         <v>25.1</v>
       </c>
-      <c r="B238" t="s">
-        <v>8</v>
+      <c r="B238">
+        <v>3</v>
       </c>
       <c r="C238">
         <v>88</v>
@@ -5157,8 +5520,8 @@
       <c r="A239" s="1">
         <v>25.4</v>
       </c>
-      <c r="B239" t="s">
-        <v>10</v>
+      <c r="B239">
+        <v>5</v>
       </c>
       <c r="C239">
         <v>77</v>
@@ -5177,8 +5540,8 @@
       <c r="A240" s="1">
         <v>25.4</v>
       </c>
-      <c r="B240" t="s">
-        <v>7</v>
+      <c r="B240">
+        <v>2</v>
       </c>
       <c r="C240">
         <v>116</v>
@@ -5197,8 +5560,8 @@
       <c r="A241" s="1">
         <v>25.5</v>
       </c>
-      <c r="B241" t="s">
-        <v>8</v>
+      <c r="B241">
+        <v>3</v>
       </c>
       <c r="C241">
         <v>96</v>
@@ -5217,8 +5580,8 @@
       <c r="A242" s="1">
         <v>25.5</v>
       </c>
-      <c r="B242" t="s">
-        <v>8</v>
+      <c r="B242">
+        <v>3</v>
       </c>
       <c r="C242">
         <v>89</v>
@@ -5237,8 +5600,8 @@
       <c r="A243" s="1">
         <v>25.8</v>
       </c>
-      <c r="B243" t="s">
-        <v>8</v>
+      <c r="B243">
+        <v>3</v>
       </c>
       <c r="C243">
         <v>92</v>
@@ -5257,8 +5620,8 @@
       <c r="A244" s="1">
         <v>26</v>
       </c>
-      <c r="B244" t="s">
-        <v>8</v>
+      <c r="B244">
+        <v>3</v>
       </c>
       <c r="C244">
         <v>46</v>
@@ -5277,8 +5640,8 @@
       <c r="A245" s="1">
         <v>26</v>
       </c>
-      <c r="B245" t="s">
-        <v>8</v>
+      <c r="B245">
+        <v>3</v>
       </c>
       <c r="C245">
         <v>113</v>
@@ -5297,8 +5660,8 @@
       <c r="A246" s="1">
         <v>26</v>
       </c>
-      <c r="B246" t="s">
-        <v>8</v>
+      <c r="B246">
+        <v>3</v>
       </c>
       <c r="C246">
         <v>70</v>
@@ -5317,8 +5680,8 @@
       <c r="A247" s="1">
         <v>26</v>
       </c>
-      <c r="B247" t="s">
-        <v>8</v>
+      <c r="B247">
+        <v>3</v>
       </c>
       <c r="C247">
         <v>69</v>
@@ -5337,8 +5700,8 @@
       <c r="A248" s="1">
         <v>26</v>
       </c>
-      <c r="B248" t="s">
-        <v>8</v>
+      <c r="B248">
+        <v>3</v>
       </c>
       <c r="C248">
         <v>46</v>
@@ -5357,8 +5720,8 @@
       <c r="A249" s="1">
         <v>26</v>
       </c>
-      <c r="B249" t="s">
-        <v>8</v>
+      <c r="B249">
+        <v>3</v>
       </c>
       <c r="C249">
         <v>90</v>
@@ -5377,8 +5740,8 @@
       <c r="A250" s="1">
         <v>26</v>
       </c>
-      <c r="B250" t="s">
-        <v>8</v>
+      <c r="B250">
+        <v>3</v>
       </c>
       <c r="C250">
         <v>80</v>
@@ -5397,8 +5760,8 @@
       <c r="A251" s="1">
         <v>26</v>
       </c>
-      <c r="B251" t="s">
-        <v>8</v>
+      <c r="B251">
+        <v>3</v>
       </c>
       <c r="C251">
         <v>67</v>
@@ -5417,8 +5780,8 @@
       <c r="A252" s="1">
         <v>26</v>
       </c>
-      <c r="B252" t="s">
-        <v>8</v>
+      <c r="B252">
+        <v>3</v>
       </c>
       <c r="C252">
         <v>78</v>
@@ -5437,8 +5800,8 @@
       <c r="A253" s="1">
         <v>26</v>
       </c>
-      <c r="B253" t="s">
-        <v>8</v>
+      <c r="B253">
+        <v>3</v>
       </c>
       <c r="C253">
         <v>75</v>
@@ -5457,8 +5820,8 @@
       <c r="A254" s="1">
         <v>26</v>
       </c>
-      <c r="B254" t="s">
-        <v>8</v>
+      <c r="B254">
+        <v>3</v>
       </c>
       <c r="C254">
         <v>93</v>
@@ -5477,8 +5840,8 @@
       <c r="A255" s="1">
         <v>26</v>
       </c>
-      <c r="B255" t="s">
-        <v>8</v>
+      <c r="B255">
+        <v>3</v>
       </c>
       <c r="C255">
         <v>79</v>
@@ -5497,8 +5860,8 @@
       <c r="A256" s="1">
         <v>26</v>
       </c>
-      <c r="B256" t="s">
-        <v>8</v>
+      <c r="B256">
+        <v>3</v>
       </c>
       <c r="C256">
         <v>75</v>
@@ -5517,8 +5880,8 @@
       <c r="A257" s="1">
         <v>26</v>
       </c>
-      <c r="B257" t="s">
-        <v>8</v>
+      <c r="B257">
+        <v>3</v>
       </c>
       <c r="C257">
         <v>92</v>
@@ -5537,8 +5900,8 @@
       <c r="A258" s="1">
         <v>26.4</v>
       </c>
-      <c r="B258" t="s">
-        <v>8</v>
+      <c r="B258">
+        <v>3</v>
       </c>
       <c r="C258">
         <v>88</v>
@@ -5557,8 +5920,8 @@
       <c r="A259" s="1">
         <v>26.5</v>
       </c>
-      <c r="B259" t="s">
-        <v>8</v>
+      <c r="B259">
+        <v>3</v>
       </c>
       <c r="C259">
         <v>72</v>
@@ -5577,8 +5940,8 @@
       <c r="A260" s="1">
         <v>26.6</v>
       </c>
-      <c r="B260" t="s">
-        <v>8</v>
+      <c r="B260">
+        <v>3</v>
       </c>
       <c r="C260">
         <v>84</v>
@@ -5597,8 +5960,8 @@
       <c r="A261" s="1">
         <v>26.6</v>
       </c>
-      <c r="B261" t="s">
-        <v>6</v>
+      <c r="B261">
+        <v>1</v>
       </c>
       <c r="C261">
         <v>105</v>
@@ -5617,8 +5980,8 @@
       <c r="A262" s="1">
         <v>26.8</v>
       </c>
-      <c r="B262" t="s">
-        <v>7</v>
+      <c r="B262">
+        <v>2</v>
       </c>
       <c r="C262">
         <v>115</v>
@@ -5637,8 +6000,8 @@
       <c r="A263" s="1">
         <v>27</v>
       </c>
-      <c r="B263" t="s">
-        <v>8</v>
+      <c r="B263">
+        <v>3</v>
       </c>
       <c r="C263">
         <v>88</v>
@@ -5657,8 +6020,8 @@
       <c r="A264" s="1">
         <v>27</v>
       </c>
-      <c r="B264" t="s">
-        <v>8</v>
+      <c r="B264">
+        <v>3</v>
       </c>
       <c r="C264">
         <v>88</v>
@@ -5677,8 +6040,8 @@
       <c r="A265" s="1">
         <v>27</v>
       </c>
-      <c r="B265" t="s">
-        <v>8</v>
+      <c r="B265">
+        <v>3</v>
       </c>
       <c r="C265">
         <v>60</v>
@@ -5697,8 +6060,8 @@
       <c r="A266" s="1">
         <v>27</v>
       </c>
-      <c r="B266" t="s">
-        <v>8</v>
+      <c r="B266">
+        <v>3</v>
       </c>
       <c r="C266">
         <v>88</v>
@@ -5717,8 +6080,8 @@
       <c r="A267" s="1">
         <v>27</v>
       </c>
-      <c r="B267" t="s">
-        <v>8</v>
+      <c r="B267">
+        <v>3</v>
       </c>
       <c r="C267">
         <v>83</v>
@@ -5737,8 +6100,8 @@
       <c r="A268" s="1">
         <v>27</v>
       </c>
-      <c r="B268" t="s">
-        <v>8</v>
+      <c r="B268">
+        <v>3</v>
       </c>
       <c r="C268">
         <v>88</v>
@@ -5757,8 +6120,8 @@
       <c r="A269" s="1">
         <v>27</v>
       </c>
-      <c r="B269" t="s">
-        <v>8</v>
+      <c r="B269">
+        <v>3</v>
       </c>
       <c r="C269">
         <v>90</v>
@@ -5777,8 +6140,8 @@
       <c r="A270" s="1">
         <v>27</v>
       </c>
-      <c r="B270" t="s">
-        <v>8</v>
+      <c r="B270">
+        <v>3</v>
       </c>
       <c r="C270">
         <v>90</v>
@@ -5797,8 +6160,8 @@
       <c r="A271" s="1">
         <v>27</v>
       </c>
-      <c r="B271" t="s">
-        <v>8</v>
+      <c r="B271">
+        <v>3</v>
       </c>
       <c r="C271">
         <v>86</v>
@@ -5817,8 +6180,8 @@
       <c r="A272" s="1">
         <v>27.2</v>
       </c>
-      <c r="B272" t="s">
-        <v>8</v>
+      <c r="B272">
+        <v>3</v>
       </c>
       <c r="C272">
         <v>97</v>
@@ -5837,8 +6200,8 @@
       <c r="A273" s="1">
         <v>27.2</v>
       </c>
-      <c r="B273" t="s">
-        <v>8</v>
+      <c r="B273">
+        <v>3</v>
       </c>
       <c r="C273">
         <v>71</v>
@@ -5857,8 +6220,8 @@
       <c r="A274" s="1">
         <v>27.2</v>
       </c>
-      <c r="B274" t="s">
-        <v>8</v>
+      <c r="B274">
+        <v>3</v>
       </c>
       <c r="C274">
         <v>84</v>
@@ -5877,8 +6240,8 @@
       <c r="A275" s="1">
         <v>27.4</v>
       </c>
-      <c r="B275" t="s">
-        <v>8</v>
+      <c r="B275">
+        <v>3</v>
       </c>
       <c r="C275">
         <v>80</v>
@@ -5897,8 +6260,8 @@
       <c r="A276" s="1">
         <v>27.5</v>
       </c>
-      <c r="B276" t="s">
-        <v>8</v>
+      <c r="B276">
+        <v>3</v>
       </c>
       <c r="C276">
         <v>95</v>
@@ -5917,8 +6280,8 @@
       <c r="A277" s="1">
         <v>27.9</v>
       </c>
-      <c r="B277" t="s">
-        <v>8</v>
+      <c r="B277">
+        <v>3</v>
       </c>
       <c r="C277">
         <v>105</v>
@@ -5937,8 +6300,8 @@
       <c r="A278" s="1">
         <v>28</v>
       </c>
-      <c r="B278" t="s">
-        <v>8</v>
+      <c r="B278">
+        <v>3</v>
       </c>
       <c r="C278">
         <v>90</v>
@@ -5957,8 +6320,8 @@
       <c r="A279" s="1">
         <v>28</v>
       </c>
-      <c r="B279" t="s">
-        <v>8</v>
+      <c r="B279">
+        <v>3</v>
       </c>
       <c r="C279">
         <v>90</v>
@@ -5977,8 +6340,8 @@
       <c r="A280" s="1">
         <v>28</v>
       </c>
-      <c r="B280" t="s">
-        <v>8</v>
+      <c r="B280">
+        <v>3</v>
       </c>
       <c r="C280">
         <v>92</v>
@@ -5997,8 +6360,8 @@
       <c r="A281" s="1">
         <v>28</v>
       </c>
-      <c r="B281" t="s">
-        <v>8</v>
+      <c r="B281">
+        <v>3</v>
       </c>
       <c r="C281">
         <v>80</v>
@@ -6017,8 +6380,8 @@
       <c r="A282" s="1">
         <v>28</v>
       </c>
-      <c r="B282" t="s">
-        <v>8</v>
+      <c r="B282">
+        <v>3</v>
       </c>
       <c r="C282">
         <v>75</v>
@@ -6037,8 +6400,8 @@
       <c r="A283" s="1">
         <v>28</v>
       </c>
-      <c r="B283" t="s">
-        <v>8</v>
+      <c r="B283">
+        <v>3</v>
       </c>
       <c r="C283">
         <v>86</v>
@@ -6057,8 +6420,8 @@
       <c r="A284" s="1">
         <v>28</v>
       </c>
-      <c r="B284" t="s">
-        <v>8</v>
+      <c r="B284">
+        <v>3</v>
       </c>
       <c r="C284">
         <v>75</v>
@@ -6077,8 +6440,8 @@
       <c r="A285" s="1">
         <v>28</v>
       </c>
-      <c r="B285" t="s">
-        <v>8</v>
+      <c r="B285">
+        <v>3</v>
       </c>
       <c r="C285">
         <v>90</v>
@@ -6097,8 +6460,8 @@
       <c r="A286" s="1">
         <v>28</v>
       </c>
-      <c r="B286" t="s">
-        <v>8</v>
+      <c r="B286">
+        <v>3</v>
       </c>
       <c r="C286">
         <v>88</v>
@@ -6117,8 +6480,8 @@
       <c r="A287" s="1">
         <v>28</v>
       </c>
-      <c r="B287" t="s">
-        <v>8</v>
+      <c r="B287">
+        <v>3</v>
       </c>
       <c r="C287">
         <v>79</v>
@@ -6137,8 +6500,8 @@
       <c r="A288" s="1">
         <v>28.1</v>
       </c>
-      <c r="B288" t="s">
-        <v>8</v>
+      <c r="B288">
+        <v>3</v>
       </c>
       <c r="C288">
         <v>80</v>
@@ -6157,8 +6520,8 @@
       <c r="A289" s="1">
         <v>28.4</v>
       </c>
-      <c r="B289" t="s">
-        <v>8</v>
+      <c r="B289">
+        <v>3</v>
       </c>
       <c r="C289">
         <v>90</v>
@@ -6177,8 +6540,8 @@
       <c r="A290" s="1">
         <v>28.8</v>
       </c>
-      <c r="B290" t="s">
-        <v>7</v>
+      <c r="B290">
+        <v>2</v>
       </c>
       <c r="C290">
         <v>115</v>
@@ -6197,8 +6560,8 @@
       <c r="A291" s="1">
         <v>29</v>
       </c>
-      <c r="B291" t="s">
-        <v>8</v>
+      <c r="B291">
+        <v>3</v>
       </c>
       <c r="C291">
         <v>49</v>
@@ -6217,8 +6580,8 @@
       <c r="A292" s="1">
         <v>29</v>
       </c>
-      <c r="B292" t="s">
-        <v>8</v>
+      <c r="B292">
+        <v>3</v>
       </c>
       <c r="C292">
         <v>83</v>
@@ -6237,8 +6600,8 @@
       <c r="A293" s="1">
         <v>29</v>
       </c>
-      <c r="B293" t="s">
-        <v>8</v>
+      <c r="B293">
+        <v>3</v>
       </c>
       <c r="C293">
         <v>75</v>
@@ -6257,8 +6620,8 @@
       <c r="A294" s="1">
         <v>29</v>
       </c>
-      <c r="B294" t="s">
-        <v>8</v>
+      <c r="B294">
+        <v>3</v>
       </c>
       <c r="C294">
         <v>70</v>
@@ -6277,8 +6640,8 @@
       <c r="A295" s="1">
         <v>29</v>
       </c>
-      <c r="B295" t="s">
-        <v>8</v>
+      <c r="B295">
+        <v>3</v>
       </c>
       <c r="C295">
         <v>52</v>
@@ -6297,8 +6660,8 @@
       <c r="A296" s="1">
         <v>29</v>
       </c>
-      <c r="B296" t="s">
-        <v>8</v>
+      <c r="B296">
+        <v>3</v>
       </c>
       <c r="C296">
         <v>70</v>
@@ -6317,8 +6680,8 @@
       <c r="A297" s="1">
         <v>29</v>
       </c>
-      <c r="B297" t="s">
-        <v>8</v>
+      <c r="B297">
+        <v>3</v>
       </c>
       <c r="C297">
         <v>78</v>
@@ -6337,8 +6700,8 @@
       <c r="A298" s="1">
         <v>29</v>
       </c>
-      <c r="B298" t="s">
-        <v>8</v>
+      <c r="B298">
+        <v>3</v>
       </c>
       <c r="C298">
         <v>84</v>
@@ -6357,8 +6720,8 @@
       <c r="A299" s="1">
         <v>29.5</v>
       </c>
-      <c r="B299" t="s">
-        <v>8</v>
+      <c r="B299">
+        <v>3</v>
       </c>
       <c r="C299">
         <v>71</v>
@@ -6377,8 +6740,8 @@
       <c r="A300" s="1">
         <v>29.5</v>
       </c>
-      <c r="B300" t="s">
-        <v>8</v>
+      <c r="B300">
+        <v>3</v>
       </c>
       <c r="C300">
         <v>68</v>
@@ -6397,8 +6760,8 @@
       <c r="A301" s="1">
         <v>29.8</v>
       </c>
-      <c r="B301" t="s">
-        <v>8</v>
+      <c r="B301">
+        <v>3</v>
       </c>
       <c r="C301">
         <v>90</v>
@@ -6417,8 +6780,8 @@
       <c r="A302" s="1">
         <v>29.8</v>
       </c>
-      <c r="B302" t="s">
-        <v>8</v>
+      <c r="B302">
+        <v>3</v>
       </c>
       <c r="C302">
         <v>62</v>
@@ -6437,8 +6800,8 @@
       <c r="A303" s="1">
         <v>29.9</v>
       </c>
-      <c r="B303" t="s">
-        <v>8</v>
+      <c r="B303">
+        <v>3</v>
       </c>
       <c r="C303">
         <v>65</v>
@@ -6457,8 +6820,8 @@
       <c r="A304" s="1">
         <v>30</v>
       </c>
-      <c r="B304" t="s">
-        <v>8</v>
+      <c r="B304">
+        <v>3</v>
       </c>
       <c r="C304">
         <v>70</v>
@@ -6477,8 +6840,8 @@
       <c r="A305" s="1">
         <v>30</v>
       </c>
-      <c r="B305" t="s">
-        <v>8</v>
+      <c r="B305">
+        <v>3</v>
       </c>
       <c r="C305">
         <v>76</v>
@@ -6497,8 +6860,8 @@
       <c r="A306" s="1">
         <v>30</v>
       </c>
-      <c r="B306" t="s">
-        <v>8</v>
+      <c r="B306">
+        <v>3</v>
       </c>
       <c r="C306">
         <v>80</v>
@@ -6517,8 +6880,8 @@
       <c r="A307" s="1">
         <v>30</v>
       </c>
-      <c r="B307" t="s">
-        <v>8</v>
+      <c r="B307">
+        <v>3</v>
       </c>
       <c r="C307">
         <v>67</v>
@@ -6537,8 +6900,8 @@
       <c r="A308" s="1">
         <v>30</v>
       </c>
-      <c r="B308" t="s">
-        <v>8</v>
+      <c r="B308">
+        <v>3</v>
       </c>
       <c r="C308">
         <v>68</v>
@@ -6557,8 +6920,8 @@
       <c r="A309" s="1">
         <v>30</v>
       </c>
-      <c r="B309" t="s">
-        <v>8</v>
+      <c r="B309">
+        <v>3</v>
       </c>
       <c r="C309">
         <v>67</v>
@@ -6577,8 +6940,8 @@
       <c r="A310" s="1">
         <v>30</v>
       </c>
-      <c r="B310" t="s">
-        <v>8</v>
+      <c r="B310">
+        <v>3</v>
       </c>
       <c r="C310">
         <v>84</v>
@@ -6597,8 +6960,8 @@
       <c r="A311" s="1">
         <v>30.5</v>
       </c>
-      <c r="B311" t="s">
-        <v>8</v>
+      <c r="B311">
+        <v>3</v>
       </c>
       <c r="C311">
         <v>63</v>
@@ -6617,8 +6980,8 @@
       <c r="A312" s="1">
         <v>30.5</v>
       </c>
-      <c r="B312" t="s">
-        <v>8</v>
+      <c r="B312">
+        <v>3</v>
       </c>
       <c r="C312">
         <v>78</v>
@@ -6637,8 +7000,8 @@
       <c r="A313" s="1">
         <v>30.7</v>
       </c>
-      <c r="B313" t="s">
-        <v>7</v>
+      <c r="B313">
+        <v>2</v>
       </c>
       <c r="C313">
         <v>76</v>
@@ -6657,8 +7020,8 @@
       <c r="A314" s="1">
         <v>30.9</v>
       </c>
-      <c r="B314" t="s">
-        <v>8</v>
+      <c r="B314">
+        <v>3</v>
       </c>
       <c r="C314">
         <v>75</v>
@@ -6677,8 +7040,8 @@
       <c r="A315" s="1">
         <v>31</v>
       </c>
-      <c r="B315" t="s">
-        <v>8</v>
+      <c r="B315">
+        <v>3</v>
       </c>
       <c r="C315">
         <v>65</v>
@@ -6697,8 +7060,8 @@
       <c r="A316" s="1">
         <v>31</v>
       </c>
-      <c r="B316" t="s">
-        <v>8</v>
+      <c r="B316">
+        <v>3</v>
       </c>
       <c r="C316">
         <v>67</v>
@@ -6717,8 +7080,8 @@
       <c r="A317" s="1">
         <v>31</v>
       </c>
-      <c r="B317" t="s">
-        <v>8</v>
+      <c r="B317">
+        <v>3</v>
       </c>
       <c r="C317">
         <v>52</v>
@@ -6737,8 +7100,8 @@
       <c r="A318" s="1">
         <v>31</v>
       </c>
-      <c r="B318" t="s">
-        <v>8</v>
+      <c r="B318">
+        <v>3</v>
       </c>
       <c r="C318">
         <v>67</v>
@@ -6757,8 +7120,8 @@
       <c r="A319" s="1">
         <v>31</v>
       </c>
-      <c r="B319" t="s">
-        <v>8</v>
+      <c r="B319">
+        <v>3</v>
       </c>
       <c r="C319">
         <v>85</v>
@@ -6777,8 +7140,8 @@
       <c r="A320" s="1">
         <v>31</v>
       </c>
-      <c r="B320" t="s">
-        <v>8</v>
+      <c r="B320">
+        <v>3</v>
       </c>
       <c r="C320">
         <v>68</v>
@@ -6797,8 +7160,8 @@
       <c r="A321" s="1">
         <v>31</v>
       </c>
-      <c r="B321" t="s">
-        <v>8</v>
+      <c r="B321">
+        <v>3</v>
       </c>
       <c r="C321">
         <v>82</v>
@@ -6817,8 +7180,8 @@
       <c r="A322" s="1">
         <v>31.3</v>
       </c>
-      <c r="B322" t="s">
-        <v>8</v>
+      <c r="B322">
+        <v>3</v>
       </c>
       <c r="C322">
         <v>75</v>
@@ -6837,8 +7200,8 @@
       <c r="A323" s="1">
         <v>31.5</v>
       </c>
-      <c r="B323" t="s">
-        <v>8</v>
+      <c r="B323">
+        <v>3</v>
       </c>
       <c r="C323">
         <v>68</v>
@@ -6857,8 +7220,8 @@
       <c r="A324" s="1">
         <v>31.5</v>
       </c>
-      <c r="B324" t="s">
-        <v>8</v>
+      <c r="B324">
+        <v>3</v>
       </c>
       <c r="C324">
         <v>71</v>
@@ -6877,8 +7240,8 @@
       <c r="A325" s="1">
         <v>31.6</v>
       </c>
-      <c r="B325" t="s">
-        <v>8</v>
+      <c r="B325">
+        <v>3</v>
       </c>
       <c r="C325">
         <v>74</v>
@@ -6897,8 +7260,8 @@
       <c r="A326" s="1">
         <v>31.8</v>
       </c>
-      <c r="B326" t="s">
-        <v>8</v>
+      <c r="B326">
+        <v>3</v>
       </c>
       <c r="C326">
         <v>65</v>
@@ -6917,8 +7280,8 @@
       <c r="A327" s="1">
         <v>31.9</v>
       </c>
-      <c r="B327" t="s">
-        <v>8</v>
+      <c r="B327">
+        <v>3</v>
       </c>
       <c r="C327">
         <v>71</v>
@@ -6937,8 +7300,8 @@
       <c r="A328" s="1">
         <v>32</v>
       </c>
-      <c r="B328" t="s">
-        <v>8</v>
+      <c r="B328">
+        <v>3</v>
       </c>
       <c r="C328">
         <v>65</v>
@@ -6957,8 +7320,8 @@
       <c r="A329" s="1">
         <v>32</v>
       </c>
-      <c r="B329" t="s">
-        <v>8</v>
+      <c r="B329">
+        <v>3</v>
       </c>
       <c r="C329">
         <v>61</v>
@@ -6977,8 +7340,8 @@
       <c r="A330" s="1">
         <v>32</v>
       </c>
-      <c r="B330" t="s">
-        <v>8</v>
+      <c r="B330">
+        <v>3</v>
       </c>
       <c r="C330">
         <v>70</v>
@@ -6997,8 +7360,8 @@
       <c r="A331" s="1">
         <v>32</v>
       </c>
-      <c r="B331" t="s">
-        <v>8</v>
+      <c r="B331">
+        <v>3</v>
       </c>
       <c r="C331">
         <v>67</v>
@@ -7017,8 +7380,8 @@
       <c r="A332" s="1">
         <v>32</v>
       </c>
-      <c r="B332" t="s">
-        <v>8</v>
+      <c r="B332">
+        <v>3</v>
       </c>
       <c r="C332">
         <v>96</v>
@@ -7037,8 +7400,8 @@
       <c r="A333" s="1">
         <v>32</v>
       </c>
-      <c r="B333" t="s">
-        <v>8</v>
+      <c r="B333">
+        <v>3</v>
       </c>
       <c r="C333">
         <v>84</v>
@@ -7057,8 +7420,8 @@
       <c r="A334" s="1">
         <v>32.1</v>
       </c>
-      <c r="B334" t="s">
-        <v>8</v>
+      <c r="B334">
+        <v>3</v>
       </c>
       <c r="C334">
         <v>70</v>
@@ -7077,8 +7440,8 @@
       <c r="A335" s="1">
         <v>32.200000000000003</v>
       </c>
-      <c r="B335" t="s">
-        <v>8</v>
+      <c r="B335">
+        <v>3</v>
       </c>
       <c r="C335">
         <v>75</v>
@@ -7097,8 +7460,8 @@
       <c r="A336" s="1">
         <v>32.299999999999997</v>
       </c>
-      <c r="B336" t="s">
-        <v>8</v>
+      <c r="B336">
+        <v>3</v>
       </c>
       <c r="C336">
         <v>67</v>
@@ -7117,8 +7480,8 @@
       <c r="A337" s="1">
         <v>32.4</v>
       </c>
-      <c r="B337" t="s">
-        <v>8</v>
+      <c r="B337">
+        <v>3</v>
       </c>
       <c r="C337">
         <v>72</v>
@@ -7137,8 +7500,8 @@
       <c r="A338" s="1">
         <v>32.4</v>
       </c>
-      <c r="B338" t="s">
-        <v>8</v>
+      <c r="B338">
+        <v>3</v>
       </c>
       <c r="C338">
         <v>75</v>
@@ -7157,8 +7520,8 @@
       <c r="A339" s="1">
         <v>32.700000000000003</v>
       </c>
-      <c r="B339" t="s">
-        <v>7</v>
+      <c r="B339">
+        <v>2</v>
       </c>
       <c r="C339">
         <v>132</v>
@@ -7177,8 +7540,8 @@
       <c r="A340" s="1">
         <v>32.799999999999997</v>
       </c>
-      <c r="B340" t="s">
-        <v>8</v>
+      <c r="B340">
+        <v>3</v>
       </c>
       <c r="C340">
         <v>52</v>
@@ -7197,8 +7560,8 @@
       <c r="A341" s="1">
         <v>32.9</v>
       </c>
-      <c r="B341" t="s">
-        <v>8</v>
+      <c r="B341">
+        <v>3</v>
       </c>
       <c r="C341">
         <v>100</v>
@@ -7217,8 +7580,8 @@
       <c r="A342" s="1">
         <v>33</v>
       </c>
-      <c r="B342" t="s">
-        <v>8</v>
+      <c r="B342">
+        <v>3</v>
       </c>
       <c r="C342">
         <v>53</v>
@@ -7237,8 +7600,8 @@
       <c r="A343" s="1">
         <v>33</v>
       </c>
-      <c r="B343" t="s">
-        <v>8</v>
+      <c r="B343">
+        <v>3</v>
       </c>
       <c r="C343">
         <v>53</v>
@@ -7257,8 +7620,8 @@
       <c r="A344" s="1">
         <v>33</v>
       </c>
-      <c r="B344" t="s">
-        <v>8</v>
+      <c r="B344">
+        <v>3</v>
       </c>
       <c r="C344">
         <v>74</v>
@@ -7277,8 +7640,8 @@
       <c r="A345" s="1">
         <v>33.5</v>
       </c>
-      <c r="B345" t="s">
-        <v>8</v>
+      <c r="B345">
+        <v>3</v>
       </c>
       <c r="C345">
         <v>70</v>
@@ -7297,8 +7660,8 @@
       <c r="A346" s="1">
         <v>33.5</v>
       </c>
-      <c r="B346" t="s">
-        <v>8</v>
+      <c r="B346">
+        <v>3</v>
       </c>
       <c r="C346">
         <v>83</v>
@@ -7317,8 +7680,8 @@
       <c r="A347" s="1">
         <v>33.5</v>
       </c>
-      <c r="B347" t="s">
-        <v>8</v>
+      <c r="B347">
+        <v>3</v>
       </c>
       <c r="C347">
         <v>90</v>
@@ -7337,8 +7700,8 @@
       <c r="A348" s="1">
         <v>33.700000000000003</v>
       </c>
-      <c r="B348" t="s">
-        <v>8</v>
+      <c r="B348">
+        <v>3</v>
       </c>
       <c r="C348">
         <v>75</v>
@@ -7357,8 +7720,8 @@
       <c r="A349" s="1">
         <v>33.799999999999997</v>
       </c>
-      <c r="B349" t="s">
-        <v>8</v>
+      <c r="B349">
+        <v>3</v>
       </c>
       <c r="C349">
         <v>67</v>
@@ -7377,8 +7740,8 @@
       <c r="A350" s="1">
         <v>34</v>
       </c>
-      <c r="B350" t="s">
-        <v>8</v>
+      <c r="B350">
+        <v>3</v>
       </c>
       <c r="C350">
         <v>88</v>
@@ -7397,8 +7760,8 @@
       <c r="A351" s="1">
         <v>34</v>
       </c>
-      <c r="B351" t="s">
-        <v>8</v>
+      <c r="B351">
+        <v>3</v>
       </c>
       <c r="C351">
         <v>70</v>
@@ -7417,8 +7780,8 @@
       <c r="A352" s="1">
         <v>34.1</v>
       </c>
-      <c r="B352" t="s">
-        <v>8</v>
+      <c r="B352">
+        <v>3</v>
       </c>
       <c r="C352">
         <v>65</v>
@@ -7437,8 +7800,8 @@
       <c r="A353" s="1">
         <v>34.1</v>
       </c>
-      <c r="B353" t="s">
-        <v>8</v>
+      <c r="B353">
+        <v>3</v>
       </c>
       <c r="C353">
         <v>68</v>
@@ -7457,8 +7820,8 @@
       <c r="A354" s="1">
         <v>34.200000000000003</v>
       </c>
-      <c r="B354" t="s">
-        <v>8</v>
+      <c r="B354">
+        <v>3</v>
       </c>
       <c r="C354">
         <v>70</v>
@@ -7477,8 +7840,8 @@
       <c r="A355" s="1">
         <v>34.299999999999997</v>
       </c>
-      <c r="B355" t="s">
-        <v>8</v>
+      <c r="B355">
+        <v>3</v>
       </c>
       <c r="C355">
         <v>78</v>
@@ -7497,8 +7860,8 @@
       <c r="A356" s="1">
         <v>34.4</v>
       </c>
-      <c r="B356" t="s">
-        <v>8</v>
+      <c r="B356">
+        <v>3</v>
       </c>
       <c r="C356">
         <v>65</v>
@@ -7517,8 +7880,8 @@
       <c r="A357" s="1">
         <v>34.5</v>
       </c>
-      <c r="B357" t="s">
-        <v>8</v>
+      <c r="B357">
+        <v>3</v>
       </c>
       <c r="C357">
         <v>70</v>
@@ -7537,8 +7900,8 @@
       <c r="A358" s="1">
         <v>34.700000000000003</v>
       </c>
-      <c r="B358" t="s">
-        <v>8</v>
+      <c r="B358">
+        <v>3</v>
       </c>
       <c r="C358">
         <v>63</v>
@@ -7557,8 +7920,8 @@
       <c r="A359" s="1">
         <v>35</v>
       </c>
-      <c r="B359" t="s">
-        <v>8</v>
+      <c r="B359">
+        <v>3</v>
       </c>
       <c r="C359">
         <v>69</v>
@@ -7577,8 +7940,8 @@
       <c r="A360" s="1">
         <v>35</v>
       </c>
-      <c r="B360" t="s">
-        <v>8</v>
+      <c r="B360">
+        <v>3</v>
       </c>
       <c r="C360">
         <v>88</v>
@@ -7597,8 +7960,8 @@
       <c r="A361" s="1">
         <v>35.1</v>
       </c>
-      <c r="B361" t="s">
-        <v>8</v>
+      <c r="B361">
+        <v>3</v>
       </c>
       <c r="C361">
         <v>60</v>
@@ -7617,8 +7980,8 @@
       <c r="A362" s="1">
         <v>35.700000000000003</v>
       </c>
-      <c r="B362" t="s">
-        <v>8</v>
+      <c r="B362">
+        <v>3</v>
       </c>
       <c r="C362">
         <v>80</v>
@@ -7637,8 +8000,8 @@
       <c r="A363" s="1">
         <v>36</v>
       </c>
-      <c r="B363" t="s">
-        <v>8</v>
+      <c r="B363">
+        <v>3</v>
       </c>
       <c r="C363">
         <v>58</v>
@@ -7657,8 +8020,8 @@
       <c r="A364" s="1">
         <v>36</v>
       </c>
-      <c r="B364" t="s">
-        <v>8</v>
+      <c r="B364">
+        <v>3</v>
       </c>
       <c r="C364">
         <v>74</v>
@@ -7677,8 +8040,8 @@
       <c r="A365" s="1">
         <v>36</v>
       </c>
-      <c r="B365" t="s">
-        <v>8</v>
+      <c r="B365">
+        <v>3</v>
       </c>
       <c r="C365">
         <v>70</v>
@@ -7697,8 +8060,8 @@
       <c r="A366" s="1">
         <v>36</v>
       </c>
-      <c r="B366" t="s">
-        <v>8</v>
+      <c r="B366">
+        <v>3</v>
       </c>
       <c r="C366">
         <v>88</v>
@@ -7717,8 +8080,8 @@
       <c r="A367" s="1">
         <v>36</v>
       </c>
-      <c r="B367" t="s">
-        <v>8</v>
+      <c r="B367">
+        <v>3</v>
       </c>
       <c r="C367">
         <v>75</v>
@@ -7737,8 +8100,8 @@
       <c r="A368" s="1">
         <v>36</v>
       </c>
-      <c r="B368" t="s">
-        <v>8</v>
+      <c r="B368">
+        <v>3</v>
       </c>
       <c r="C368">
         <v>84</v>
@@ -7757,8 +8120,8 @@
       <c r="A369" s="1">
         <v>36.1</v>
       </c>
-      <c r="B369" t="s">
-        <v>8</v>
+      <c r="B369">
+        <v>3</v>
       </c>
       <c r="C369">
         <v>66</v>
@@ -7777,8 +8140,8 @@
       <c r="A370" s="1">
         <v>36.1</v>
       </c>
-      <c r="B370" t="s">
-        <v>8</v>
+      <c r="B370">
+        <v>3</v>
       </c>
       <c r="C370">
         <v>60</v>
@@ -7797,8 +8160,8 @@
       <c r="A371" s="1">
         <v>36.4</v>
       </c>
-      <c r="B371" t="s">
-        <v>10</v>
+      <c r="B371">
+        <v>5</v>
       </c>
       <c r="C371">
         <v>67</v>
@@ -7817,8 +8180,8 @@
       <c r="A372" s="1">
         <v>37</v>
       </c>
-      <c r="B372" t="s">
-        <v>8</v>
+      <c r="B372">
+        <v>3</v>
       </c>
       <c r="C372">
         <v>92</v>
@@ -7837,8 +8200,8 @@
       <c r="A373" s="1">
         <v>37</v>
       </c>
-      <c r="B373" t="s">
-        <v>8</v>
+      <c r="B373">
+        <v>3</v>
       </c>
       <c r="C373">
         <v>65</v>
@@ -7857,8 +8220,8 @@
       <c r="A374" s="1">
         <v>37</v>
       </c>
-      <c r="B374" t="s">
-        <v>8</v>
+      <c r="B374">
+        <v>3</v>
       </c>
       <c r="C374">
         <v>68</v>
@@ -7877,8 +8240,8 @@
       <c r="A375" s="1">
         <v>37.200000000000003</v>
       </c>
-      <c r="B375" t="s">
-        <v>8</v>
+      <c r="B375">
+        <v>3</v>
       </c>
       <c r="C375">
         <v>65</v>
@@ -7897,8 +8260,8 @@
       <c r="A376" s="1">
         <v>37.299999999999997</v>
       </c>
-      <c r="B376" t="s">
-        <v>8</v>
+      <c r="B376">
+        <v>3</v>
       </c>
       <c r="C376">
         <v>69</v>
@@ -7917,8 +8280,8 @@
       <c r="A377" s="1">
         <v>37.700000000000003</v>
       </c>
-      <c r="B377" t="s">
-        <v>8</v>
+      <c r="B377">
+        <v>3</v>
       </c>
       <c r="C377">
         <v>62</v>
@@ -7937,8 +8300,8 @@
       <c r="A378" s="1">
         <v>38</v>
       </c>
-      <c r="B378" t="s">
-        <v>8</v>
+      <c r="B378">
+        <v>3</v>
       </c>
       <c r="C378">
         <v>63</v>
@@ -7957,8 +8320,8 @@
       <c r="A379" s="1">
         <v>38</v>
       </c>
-      <c r="B379" t="s">
-        <v>8</v>
+      <c r="B379">
+        <v>3</v>
       </c>
       <c r="C379">
         <v>67</v>
@@ -7977,8 +8340,8 @@
       <c r="A380" s="1">
         <v>38</v>
       </c>
-      <c r="B380" t="s">
-        <v>8</v>
+      <c r="B380">
+        <v>3</v>
       </c>
       <c r="C380">
         <v>67</v>
@@ -7997,8 +8360,8 @@
       <c r="A381" s="1">
         <v>38</v>
       </c>
-      <c r="B381" t="s">
-        <v>7</v>
+      <c r="B381">
+        <v>2</v>
       </c>
       <c r="C381">
         <v>85</v>
@@ -8017,8 +8380,8 @@
       <c r="A382" s="1">
         <v>38.1</v>
       </c>
-      <c r="B382" t="s">
-        <v>8</v>
+      <c r="B382">
+        <v>3</v>
       </c>
       <c r="C382">
         <v>60</v>
@@ -8037,8 +8400,8 @@
       <c r="A383" s="1">
         <v>39</v>
       </c>
-      <c r="B383" t="s">
-        <v>8</v>
+      <c r="B383">
+        <v>3</v>
       </c>
       <c r="C383">
         <v>64</v>
@@ -8057,8 +8420,8 @@
       <c r="A384" s="1">
         <v>39.1</v>
       </c>
-      <c r="B384" t="s">
-        <v>8</v>
+      <c r="B384">
+        <v>3</v>
       </c>
       <c r="C384">
         <v>58</v>
@@ -8077,8 +8440,8 @@
       <c r="A385" s="1">
         <v>39.4</v>
       </c>
-      <c r="B385" t="s">
-        <v>8</v>
+      <c r="B385">
+        <v>3</v>
       </c>
       <c r="C385">
         <v>70</v>
@@ -8097,8 +8460,8 @@
       <c r="A386" s="1">
         <v>40.799999999999997</v>
       </c>
-      <c r="B386" t="s">
-        <v>8</v>
+      <c r="B386">
+        <v>3</v>
       </c>
       <c r="C386">
         <v>65</v>
@@ -8117,8 +8480,8 @@
       <c r="A387" s="1">
         <v>41.5</v>
       </c>
-      <c r="B387" t="s">
-        <v>8</v>
+      <c r="B387">
+        <v>3</v>
       </c>
       <c r="C387">
         <v>76</v>
@@ -8137,8 +8500,8 @@
       <c r="A388" s="1">
         <v>43.1</v>
       </c>
-      <c r="B388" t="s">
-        <v>8</v>
+      <c r="B388">
+        <v>3</v>
       </c>
       <c r="C388">
         <v>48</v>
@@ -8157,8 +8520,8 @@
       <c r="A389" s="1">
         <v>43.4</v>
       </c>
-      <c r="B389" t="s">
-        <v>8</v>
+      <c r="B389">
+        <v>3</v>
       </c>
       <c r="C389">
         <v>48</v>
@@ -8177,8 +8540,8 @@
       <c r="A390" s="1">
         <v>44</v>
       </c>
-      <c r="B390" t="s">
-        <v>8</v>
+      <c r="B390">
+        <v>3</v>
       </c>
       <c r="C390">
         <v>52</v>
@@ -8197,8 +8560,8 @@
       <c r="A391" s="1">
         <v>44.3</v>
       </c>
-      <c r="B391" t="s">
-        <v>8</v>
+      <c r="B391">
+        <v>3</v>
       </c>
       <c r="C391">
         <v>48</v>
@@ -8217,8 +8580,8 @@
       <c r="A392" s="1">
         <v>44.6</v>
       </c>
-      <c r="B392" t="s">
-        <v>8</v>
+      <c r="B392">
+        <v>3</v>
       </c>
       <c r="C392">
         <v>67</v>
@@ -8237,8 +8600,8 @@
       <c r="A393" s="1">
         <v>46.6</v>
       </c>
-      <c r="B393" t="s">
-        <v>8</v>
+      <c r="B393">
+        <v>3</v>
       </c>
       <c r="C393">
         <v>65</v>

</xml_diff>